<commit_message>
updates catch, release, recapture tables from grant 12-15-2022
</commit_message>
<xml_diff>
--- a/data-raw/butte_recapture_edi.xlsx
+++ b/data-raw/butte_recapture_edi.xlsx
@@ -8,7 +8,11 @@
   </bookViews>
   <sheets>
     <sheet sheetId="1" r:id="rId1" name="Recapture EDI"/>
+    <sheet r:id="rId4" name="Recapture_EDI" sheetId="2"/>
   </sheets>
+  <definedNames>
+    <definedName name="Recapture_EDI">'Recapture_EDI'!$A$1:$W$27</definedName>
+  </definedNames>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
 </file>
@@ -287,6 +291,10 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="8" applyFill="1" applyProtection="1" applyBorder="1" applyAlignment="1" applyFont="1" xfId="0">
       <alignment wrapText="1" vertical="center" horizontal="general"/>
+      <protection locked="1" hidden="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyProtection="1" applyNumberFormat="1" xfId="0">
+      <alignment wrapText="0" vertical="center" horizontal="general"/>
       <protection locked="1" hidden="0"/>
     </xf>
   </cellXfs>
@@ -2882,4 +2890,2324 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:W27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row outlineLevel="0" r="1">
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>ProjectDescriptionID</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>catchRawID</t>
+        </is>
+      </c>
+      <c r="C1" s="0" t="inlineStr">
+        <is>
+          <t>trapVisitID</t>
+        </is>
+      </c>
+      <c r="D1" s="0" t="inlineStr">
+        <is>
+          <t>commonName</t>
+        </is>
+      </c>
+      <c r="E1" s="0" t="inlineStr">
+        <is>
+          <t>releaseID</t>
+        </is>
+      </c>
+      <c r="F1" s="0" t="inlineStr">
+        <is>
+          <t>atCaptureRun</t>
+        </is>
+      </c>
+      <c r="G1" s="0" t="inlineStr">
+        <is>
+          <t>finalRun</t>
+        </is>
+      </c>
+      <c r="H1" s="0" t="inlineStr">
+        <is>
+          <t>fishOrigin</t>
+        </is>
+      </c>
+      <c r="I1" s="0" t="inlineStr">
+        <is>
+          <t>lifeStage</t>
+        </is>
+      </c>
+      <c r="J1" s="0" t="inlineStr">
+        <is>
+          <t>mort</t>
+        </is>
+      </c>
+      <c r="K1" s="0" t="inlineStr">
+        <is>
+          <t>actualCount</t>
+        </is>
+      </c>
+      <c r="L1" s="0" t="inlineStr">
+        <is>
+          <t>forkLength</t>
+        </is>
+      </c>
+      <c r="M1" s="0" t="inlineStr">
+        <is>
+          <t>totalLength</t>
+        </is>
+      </c>
+      <c r="N1" s="0" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="O1" s="0" t="inlineStr">
+        <is>
+          <t>actualCountID</t>
+        </is>
+      </c>
+      <c r="P1" s="0" t="inlineStr">
+        <is>
+          <t>visitTime</t>
+        </is>
+      </c>
+      <c r="Q1" s="0" t="inlineStr">
+        <is>
+          <t>visitType</t>
+        </is>
+      </c>
+      <c r="R1" s="0" t="inlineStr">
+        <is>
+          <t>siteName</t>
+        </is>
+      </c>
+      <c r="S1" s="0" t="inlineStr">
+        <is>
+          <t>subSiteName</t>
+        </is>
+      </c>
+      <c r="T1" s="0" t="inlineStr">
+        <is>
+          <t>markType</t>
+        </is>
+      </c>
+      <c r="U1" s="0" t="inlineStr">
+        <is>
+          <t>markColor</t>
+        </is>
+      </c>
+      <c r="V1" s="0" t="inlineStr">
+        <is>
+          <t>markPosition</t>
+        </is>
+      </c>
+      <c r="W1" s="0" t="inlineStr">
+        <is>
+          <t>markCode</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="2">
+      <c r="A2" s="0">
+        <v>11</v>
+      </c>
+      <c r="B2" s="0">
+        <v>22160</v>
+      </c>
+      <c r="C2" s="0">
+        <v>1299</v>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>Chinook salmon</t>
+        </is>
+      </c>
+      <c r="E2" s="0">
+        <v>263</v>
+      </c>
+      <c r="F2" s="0" t="inlineStr">
+        <is>
+          <t>Not recorded</t>
+        </is>
+      </c>
+      <c r="H2" s="0" t="inlineStr">
+        <is>
+          <t>Natural</t>
+        </is>
+      </c>
+      <c r="I2" s="0" t="inlineStr">
+        <is>
+          <t>Not recorded</t>
+        </is>
+      </c>
+      <c r="J2" s="0" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K2" s="0" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N2" s="0">
+        <v>1</v>
+      </c>
+      <c r="O2" s="0">
+        <v>1</v>
+      </c>
+      <c r="P2" s="10">
+        <v>44213.3964236111</v>
+      </c>
+      <c r="Q2" s="0" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
+      <c r="R2" s="0" t="inlineStr">
+        <is>
+          <t>Parrot-Phelan RST</t>
+        </is>
+      </c>
+      <c r="S2" s="0" t="inlineStr">
+        <is>
+          <t>PP RST</t>
+        </is>
+      </c>
+      <c r="T2" s="0" t="inlineStr">
+        <is>
+          <t>Pigment / dye</t>
+        </is>
+      </c>
+      <c r="U2" s="0" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="V2" s="0" t="inlineStr">
+        <is>
+          <t>Whole body</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="3">
+      <c r="A3" s="0">
+        <v>11</v>
+      </c>
+      <c r="B3" s="0">
+        <v>22974</v>
+      </c>
+      <c r="C3" s="0">
+        <v>1344</v>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>Chinook salmon</t>
+        </is>
+      </c>
+      <c r="E3" s="0">
+        <v>264</v>
+      </c>
+      <c r="F3" s="0" t="inlineStr">
+        <is>
+          <t>Not recorded</t>
+        </is>
+      </c>
+      <c r="H3" s="0" t="inlineStr">
+        <is>
+          <t>Natural</t>
+        </is>
+      </c>
+      <c r="I3" s="0" t="inlineStr">
+        <is>
+          <t>Not recorded</t>
+        </is>
+      </c>
+      <c r="J3" s="0" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K3" s="0" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N3" s="0">
+        <v>10</v>
+      </c>
+      <c r="O3" s="0">
+        <v>1</v>
+      </c>
+      <c r="P3" s="10">
+        <v>44238.3755439815</v>
+      </c>
+      <c r="Q3" s="0" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
+      <c r="R3" s="0" t="inlineStr">
+        <is>
+          <t>Parrot-Phelan RST</t>
+        </is>
+      </c>
+      <c r="S3" s="0" t="inlineStr">
+        <is>
+          <t>PP RST</t>
+        </is>
+      </c>
+      <c r="T3" s="0" t="inlineStr">
+        <is>
+          <t>Pigment / dye</t>
+        </is>
+      </c>
+      <c r="U3" s="0" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="V3" s="0" t="inlineStr">
+        <is>
+          <t>Whole body</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="4">
+      <c r="A4" s="0">
+        <v>11</v>
+      </c>
+      <c r="B4" s="0">
+        <v>22989</v>
+      </c>
+      <c r="C4" s="0">
+        <v>1345</v>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>Chinook salmon</t>
+        </is>
+      </c>
+      <c r="E4" s="0">
+        <v>264</v>
+      </c>
+      <c r="F4" s="0" t="inlineStr">
+        <is>
+          <t>Not recorded</t>
+        </is>
+      </c>
+      <c r="H4" s="0" t="inlineStr">
+        <is>
+          <t>Natural</t>
+        </is>
+      </c>
+      <c r="I4" s="0" t="inlineStr">
+        <is>
+          <t>Juvenile</t>
+        </is>
+      </c>
+      <c r="J4" s="0" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K4" s="0" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N4" s="0">
+        <v>8</v>
+      </c>
+      <c r="O4" s="0">
+        <v>1</v>
+      </c>
+      <c r="P4" s="10">
+        <v>44239.6459143519</v>
+      </c>
+      <c r="Q4" s="0" t="inlineStr">
+        <is>
+          <t>Unplanned restart</t>
+        </is>
+      </c>
+      <c r="R4" s="0" t="inlineStr">
+        <is>
+          <t>Parrot-Phelan RST</t>
+        </is>
+      </c>
+      <c r="S4" s="0" t="inlineStr">
+        <is>
+          <t>PP RST</t>
+        </is>
+      </c>
+      <c r="T4" s="0" t="inlineStr">
+        <is>
+          <t>Pigment / dye</t>
+        </is>
+      </c>
+      <c r="U4" s="0" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="V4" s="0" t="inlineStr">
+        <is>
+          <t>Whole body</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="5">
+      <c r="A5" s="0">
+        <v>11</v>
+      </c>
+      <c r="B5" s="0">
+        <v>23474</v>
+      </c>
+      <c r="C5" s="0">
+        <v>1371</v>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>Chinook salmon</t>
+        </is>
+      </c>
+      <c r="E5" s="0">
+        <v>265</v>
+      </c>
+      <c r="F5" s="0" t="inlineStr">
+        <is>
+          <t>Not recorded</t>
+        </is>
+      </c>
+      <c r="H5" s="0" t="inlineStr">
+        <is>
+          <t>Natural</t>
+        </is>
+      </c>
+      <c r="I5" s="0" t="inlineStr">
+        <is>
+          <t>Juvenile</t>
+        </is>
+      </c>
+      <c r="J5" s="0" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K5" s="0" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N5" s="0">
+        <v>65</v>
+      </c>
+      <c r="O5" s="0">
+        <v>1</v>
+      </c>
+      <c r="P5" s="10">
+        <v>44252.3962037037</v>
+      </c>
+      <c r="Q5" s="0" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
+      <c r="R5" s="0" t="inlineStr">
+        <is>
+          <t>Parrot-Phelan RST</t>
+        </is>
+      </c>
+      <c r="S5" s="0" t="inlineStr">
+        <is>
+          <t>PP RST</t>
+        </is>
+      </c>
+      <c r="T5" s="0" t="inlineStr">
+        <is>
+          <t>Pigment / dye</t>
+        </is>
+      </c>
+      <c r="U5" s="0" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="V5" s="0" t="inlineStr">
+        <is>
+          <t>Whole body</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="6">
+      <c r="A6" s="0">
+        <v>11</v>
+      </c>
+      <c r="B6" s="0">
+        <v>23484</v>
+      </c>
+      <c r="C6" s="0">
+        <v>1372</v>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>Chinook salmon</t>
+        </is>
+      </c>
+      <c r="E6" s="0">
+        <v>265</v>
+      </c>
+      <c r="F6" s="0" t="inlineStr">
+        <is>
+          <t>Not recorded</t>
+        </is>
+      </c>
+      <c r="H6" s="0" t="inlineStr">
+        <is>
+          <t>Natural</t>
+        </is>
+      </c>
+      <c r="I6" s="0" t="inlineStr">
+        <is>
+          <t>Not recorded</t>
+        </is>
+      </c>
+      <c r="J6" s="0" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K6" s="0" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N6" s="0">
+        <v>24</v>
+      </c>
+      <c r="O6" s="0">
+        <v>1</v>
+      </c>
+      <c r="P6" s="10">
+        <v>44253.3755902778</v>
+      </c>
+      <c r="Q6" s="0" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
+      <c r="R6" s="0" t="inlineStr">
+        <is>
+          <t>Parrot-Phelan RST</t>
+        </is>
+      </c>
+      <c r="S6" s="0" t="inlineStr">
+        <is>
+          <t>PP RST</t>
+        </is>
+      </c>
+      <c r="T6" s="0" t="inlineStr">
+        <is>
+          <t>Pigment / dye</t>
+        </is>
+      </c>
+      <c r="U6" s="0" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="V6" s="0" t="inlineStr">
+        <is>
+          <t>Whole body</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="7">
+      <c r="A7" s="0">
+        <v>11</v>
+      </c>
+      <c r="B7" s="0">
+        <v>23804</v>
+      </c>
+      <c r="C7" s="0">
+        <v>1405</v>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>Chinook salmon</t>
+        </is>
+      </c>
+      <c r="E7" s="0">
+        <v>266</v>
+      </c>
+      <c r="F7" s="0" t="inlineStr">
+        <is>
+          <t>Spring</t>
+        </is>
+      </c>
+      <c r="H7" s="0" t="inlineStr">
+        <is>
+          <t>Natural</t>
+        </is>
+      </c>
+      <c r="I7" s="0" t="inlineStr">
+        <is>
+          <t>Juvenile</t>
+        </is>
+      </c>
+      <c r="J7" s="0" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K7" s="0" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N7" s="0">
+        <v>13</v>
+      </c>
+      <c r="O7" s="0">
+        <v>1</v>
+      </c>
+      <c r="P7" s="10">
+        <v>44266.4030324074</v>
+      </c>
+      <c r="Q7" s="0" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
+      <c r="R7" s="0" t="inlineStr">
+        <is>
+          <t>Parrot-Phelan RST</t>
+        </is>
+      </c>
+      <c r="S7" s="0" t="inlineStr">
+        <is>
+          <t>PP RST</t>
+        </is>
+      </c>
+      <c r="T7" s="0" t="inlineStr">
+        <is>
+          <t>Pigment / dye</t>
+        </is>
+      </c>
+      <c r="U7" s="0" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="V7" s="0" t="inlineStr">
+        <is>
+          <t>Whole body</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="8">
+      <c r="A8" s="0">
+        <v>11</v>
+      </c>
+      <c r="B8" s="0">
+        <v>23818</v>
+      </c>
+      <c r="C8" s="0">
+        <v>1406</v>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>Chinook salmon</t>
+        </is>
+      </c>
+      <c r="E8" s="0">
+        <v>266</v>
+      </c>
+      <c r="F8" s="0" t="inlineStr">
+        <is>
+          <t>Spring</t>
+        </is>
+      </c>
+      <c r="H8" s="0" t="inlineStr">
+        <is>
+          <t>Natural</t>
+        </is>
+      </c>
+      <c r="I8" s="0" t="inlineStr">
+        <is>
+          <t>Not recorded</t>
+        </is>
+      </c>
+      <c r="J8" s="0" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K8" s="0" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N8" s="0">
+        <v>6</v>
+      </c>
+      <c r="O8" s="0">
+        <v>1</v>
+      </c>
+      <c r="P8" s="10">
+        <v>44267.3755787037</v>
+      </c>
+      <c r="Q8" s="0" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
+      <c r="R8" s="0" t="inlineStr">
+        <is>
+          <t>Parrot-Phelan RST</t>
+        </is>
+      </c>
+      <c r="S8" s="0" t="inlineStr">
+        <is>
+          <t>PP RST</t>
+        </is>
+      </c>
+      <c r="T8" s="0" t="inlineStr">
+        <is>
+          <t>Pigment / dye</t>
+        </is>
+      </c>
+      <c r="U8" s="0" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="V8" s="0" t="inlineStr">
+        <is>
+          <t>Whole body</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="9">
+      <c r="A9" s="0">
+        <v>11</v>
+      </c>
+      <c r="B9" s="0">
+        <v>25130</v>
+      </c>
+      <c r="C9" s="0">
+        <v>1471</v>
+      </c>
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>Chinook salmon</t>
+        </is>
+      </c>
+      <c r="E9" s="0">
+        <v>267</v>
+      </c>
+      <c r="F9" s="0" t="inlineStr">
+        <is>
+          <t>Not recorded</t>
+        </is>
+      </c>
+      <c r="H9" s="0" t="inlineStr">
+        <is>
+          <t>Natural</t>
+        </is>
+      </c>
+      <c r="I9" s="0" t="inlineStr">
+        <is>
+          <t>Not recorded</t>
+        </is>
+      </c>
+      <c r="J9" s="0" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K9" s="0" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N9" s="0">
+        <v>6</v>
+      </c>
+      <c r="O9" s="0">
+        <v>1</v>
+      </c>
+      <c r="P9" s="10">
+        <v>44295.4794916088</v>
+      </c>
+      <c r="Q9" s="0" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
+      <c r="R9" s="0" t="inlineStr">
+        <is>
+          <t>Parrot-Phelan RST</t>
+        </is>
+      </c>
+      <c r="S9" s="0" t="inlineStr">
+        <is>
+          <t>PP RST</t>
+        </is>
+      </c>
+      <c r="T9" s="0" t="inlineStr">
+        <is>
+          <t>Pigment / dye</t>
+        </is>
+      </c>
+      <c r="U9" s="0" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="V9" s="0" t="inlineStr">
+        <is>
+          <t>Whole body</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="10">
+      <c r="A10" s="0">
+        <v>11</v>
+      </c>
+      <c r="B10" s="0">
+        <v>25709</v>
+      </c>
+      <c r="C10" s="0">
+        <v>1486</v>
+      </c>
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>Chinook salmon</t>
+        </is>
+      </c>
+      <c r="E10" s="0">
+        <v>268</v>
+      </c>
+      <c r="F10" s="0" t="inlineStr">
+        <is>
+          <t>Not recorded</t>
+        </is>
+      </c>
+      <c r="H10" s="0" t="inlineStr">
+        <is>
+          <t>Natural</t>
+        </is>
+      </c>
+      <c r="I10" s="0" t="inlineStr">
+        <is>
+          <t>Not recorded</t>
+        </is>
+      </c>
+      <c r="J10" s="0" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K10" s="0" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N10" s="0">
+        <v>109</v>
+      </c>
+      <c r="O10" s="0">
+        <v>1</v>
+      </c>
+      <c r="P10" s="10">
+        <v>44302.4375231481</v>
+      </c>
+      <c r="Q10" s="0" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
+      <c r="R10" s="0" t="inlineStr">
+        <is>
+          <t>Parrot-Phelan RST</t>
+        </is>
+      </c>
+      <c r="S10" s="0" t="inlineStr">
+        <is>
+          <t>PP RST</t>
+        </is>
+      </c>
+      <c r="T10" s="0" t="inlineStr">
+        <is>
+          <t>Pigment / dye</t>
+        </is>
+      </c>
+      <c r="U10" s="0" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="V10" s="0" t="inlineStr">
+        <is>
+          <t>Whole body</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="11">
+      <c r="A11" s="0">
+        <v>11</v>
+      </c>
+      <c r="B11" s="0">
+        <v>28425</v>
+      </c>
+      <c r="C11" s="0">
+        <v>1488</v>
+      </c>
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>Chinook salmon</t>
+        </is>
+      </c>
+      <c r="E11" s="0">
+        <v>268</v>
+      </c>
+      <c r="F11" s="0" t="inlineStr">
+        <is>
+          <t>Spring</t>
+        </is>
+      </c>
+      <c r="H11" s="0" t="inlineStr">
+        <is>
+          <t>Natural</t>
+        </is>
+      </c>
+      <c r="I11" s="0" t="inlineStr">
+        <is>
+          <t>Juvenile</t>
+        </is>
+      </c>
+      <c r="J11" s="0" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K11" s="0" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N11" s="0">
+        <v>3</v>
+      </c>
+      <c r="O11" s="0">
+        <v>1</v>
+      </c>
+      <c r="P11" s="10">
+        <v>44303.4665583681</v>
+      </c>
+      <c r="Q11" s="0" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
+      <c r="R11" s="0" t="inlineStr">
+        <is>
+          <t>Parrot-Phelan RST</t>
+        </is>
+      </c>
+      <c r="S11" s="0" t="inlineStr">
+        <is>
+          <t>PP RST</t>
+        </is>
+      </c>
+      <c r="T11" s="0" t="inlineStr">
+        <is>
+          <t>Pigment / dye</t>
+        </is>
+      </c>
+      <c r="U11" s="0" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="V11" s="0" t="inlineStr">
+        <is>
+          <t>Whole body</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="12">
+      <c r="A12" s="0">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0">
+        <v>28563</v>
+      </c>
+      <c r="C12" s="0">
+        <v>1281</v>
+      </c>
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>Chinook salmon</t>
+        </is>
+      </c>
+      <c r="E12" s="0">
+        <v>261</v>
+      </c>
+      <c r="F12" s="0" t="inlineStr">
+        <is>
+          <t>Spring</t>
+        </is>
+      </c>
+      <c r="H12" s="0" t="inlineStr">
+        <is>
+          <t>Natural</t>
+        </is>
+      </c>
+      <c r="I12" s="0" t="inlineStr">
+        <is>
+          <t>Fry</t>
+        </is>
+      </c>
+      <c r="J12" s="0" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K12" s="0" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N12" s="0">
+        <v>14</v>
+      </c>
+      <c r="O12" s="0">
+        <v>1</v>
+      </c>
+      <c r="P12" s="10">
+        <v>44203.4376967593</v>
+      </c>
+      <c r="Q12" s="0" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
+      <c r="R12" s="0" t="inlineStr">
+        <is>
+          <t>Parrot-Phelan RST</t>
+        </is>
+      </c>
+      <c r="S12" s="0" t="inlineStr">
+        <is>
+          <t>PP RST</t>
+        </is>
+      </c>
+      <c r="T12" s="0" t="inlineStr">
+        <is>
+          <t>Pigment / dye</t>
+        </is>
+      </c>
+      <c r="U12" s="0" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="V12" s="0" t="inlineStr">
+        <is>
+          <t>Whole body</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="13">
+      <c r="A13" s="0">
+        <v>11</v>
+      </c>
+      <c r="B13" s="0">
+        <v>29767</v>
+      </c>
+      <c r="C13" s="0">
+        <v>1283</v>
+      </c>
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>Chinook salmon</t>
+        </is>
+      </c>
+      <c r="E13" s="0">
+        <v>261</v>
+      </c>
+      <c r="F13" s="0" t="inlineStr">
+        <is>
+          <t>Not recorded</t>
+        </is>
+      </c>
+      <c r="H13" s="0" t="inlineStr">
+        <is>
+          <t>Natural</t>
+        </is>
+      </c>
+      <c r="I13" s="0" t="inlineStr">
+        <is>
+          <t>Juvenile</t>
+        </is>
+      </c>
+      <c r="J13" s="0" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K13" s="0" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N13" s="0">
+        <v>5</v>
+      </c>
+      <c r="O13" s="0">
+        <v>1</v>
+      </c>
+      <c r="P13" s="10">
+        <v>44204.3959606482</v>
+      </c>
+      <c r="Q13" s="0" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
+      <c r="R13" s="0" t="inlineStr">
+        <is>
+          <t>Parrot-Phelan RST</t>
+        </is>
+      </c>
+      <c r="S13" s="0" t="inlineStr">
+        <is>
+          <t>PP RST</t>
+        </is>
+      </c>
+      <c r="T13" s="0" t="inlineStr">
+        <is>
+          <t>Pigment / dye</t>
+        </is>
+      </c>
+      <c r="U13" s="0" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="V13" s="0" t="inlineStr">
+        <is>
+          <t>Whole body</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="14">
+      <c r="A14" s="0">
+        <v>11</v>
+      </c>
+      <c r="B14" s="0">
+        <v>29768</v>
+      </c>
+      <c r="C14" s="0">
+        <v>1285</v>
+      </c>
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>Chinook salmon</t>
+        </is>
+      </c>
+      <c r="E14" s="0">
+        <v>261</v>
+      </c>
+      <c r="F14" s="0" t="inlineStr">
+        <is>
+          <t>Not recorded</t>
+        </is>
+      </c>
+      <c r="H14" s="0" t="inlineStr">
+        <is>
+          <t>Natural</t>
+        </is>
+      </c>
+      <c r="I14" s="0" t="inlineStr">
+        <is>
+          <t>Juvenile</t>
+        </is>
+      </c>
+      <c r="J14" s="0" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K14" s="0" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N14" s="0">
+        <v>3</v>
+      </c>
+      <c r="O14" s="0">
+        <v>1</v>
+      </c>
+      <c r="P14" s="10">
+        <v>44205.416712963</v>
+      </c>
+      <c r="Q14" s="0" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
+      <c r="R14" s="0" t="inlineStr">
+        <is>
+          <t>Parrot-Phelan RST</t>
+        </is>
+      </c>
+      <c r="S14" s="0" t="inlineStr">
+        <is>
+          <t>PP RST</t>
+        </is>
+      </c>
+      <c r="T14" s="0" t="inlineStr">
+        <is>
+          <t>Pigment / dye</t>
+        </is>
+      </c>
+      <c r="U14" s="0" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="V14" s="0" t="inlineStr">
+        <is>
+          <t>Whole body</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="15">
+      <c r="A15" s="0">
+        <v>11</v>
+      </c>
+      <c r="B15" s="0">
+        <v>29770</v>
+      </c>
+      <c r="C15" s="0">
+        <v>1297</v>
+      </c>
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>Chinook salmon</t>
+        </is>
+      </c>
+      <c r="E15" s="0">
+        <v>263</v>
+      </c>
+      <c r="F15" s="0" t="inlineStr">
+        <is>
+          <t>Not recorded</t>
+        </is>
+      </c>
+      <c r="H15" s="0" t="inlineStr">
+        <is>
+          <t>Natural</t>
+        </is>
+      </c>
+      <c r="I15" s="0" t="inlineStr">
+        <is>
+          <t>Juvenile</t>
+        </is>
+      </c>
+      <c r="J15" s="0" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K15" s="0" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N15" s="0">
+        <v>55</v>
+      </c>
+      <c r="O15" s="0">
+        <v>1</v>
+      </c>
+      <c r="P15" s="10">
+        <v>44211.5833449074</v>
+      </c>
+      <c r="Q15" s="0" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
+      <c r="R15" s="0" t="inlineStr">
+        <is>
+          <t>Parrot-Phelan RST</t>
+        </is>
+      </c>
+      <c r="S15" s="0" t="inlineStr">
+        <is>
+          <t>PP RST</t>
+        </is>
+      </c>
+      <c r="T15" s="0" t="inlineStr">
+        <is>
+          <t>Pigment / dye</t>
+        </is>
+      </c>
+      <c r="U15" s="0" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="V15" s="0" t="inlineStr">
+        <is>
+          <t>Whole body</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="16">
+      <c r="A16" s="0">
+        <v>11</v>
+      </c>
+      <c r="B16" s="0">
+        <v>29771</v>
+      </c>
+      <c r="C16" s="0">
+        <v>1298</v>
+      </c>
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>Chinook salmon</t>
+        </is>
+      </c>
+      <c r="E16" s="0">
+        <v>263</v>
+      </c>
+      <c r="F16" s="0" t="inlineStr">
+        <is>
+          <t>Not recorded</t>
+        </is>
+      </c>
+      <c r="H16" s="0" t="inlineStr">
+        <is>
+          <t>Natural</t>
+        </is>
+      </c>
+      <c r="I16" s="0" t="inlineStr">
+        <is>
+          <t>Juvenile</t>
+        </is>
+      </c>
+      <c r="J16" s="0" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K16" s="0" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N16" s="0">
+        <v>5</v>
+      </c>
+      <c r="O16" s="0">
+        <v>1</v>
+      </c>
+      <c r="P16" s="10">
+        <v>44212.3750462963</v>
+      </c>
+      <c r="Q16" s="0" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
+      <c r="R16" s="0" t="inlineStr">
+        <is>
+          <t>Parrot-Phelan RST</t>
+        </is>
+      </c>
+      <c r="S16" s="0" t="inlineStr">
+        <is>
+          <t>PP RST</t>
+        </is>
+      </c>
+      <c r="T16" s="0" t="inlineStr">
+        <is>
+          <t>Pigment / dye</t>
+        </is>
+      </c>
+      <c r="U16" s="0" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="V16" s="0" t="inlineStr">
+        <is>
+          <t>Whole body</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="17">
+      <c r="A17" s="0">
+        <v>11</v>
+      </c>
+      <c r="B17" s="0">
+        <v>32454</v>
+      </c>
+      <c r="C17" s="0">
+        <v>1781</v>
+      </c>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>Chinook salmon</t>
+        </is>
+      </c>
+      <c r="E17" s="0">
+        <v>269</v>
+      </c>
+      <c r="F17" s="0" t="inlineStr">
+        <is>
+          <t>Spring</t>
+        </is>
+      </c>
+      <c r="H17" s="0" t="inlineStr">
+        <is>
+          <t>Natural</t>
+        </is>
+      </c>
+      <c r="I17" s="0" t="inlineStr">
+        <is>
+          <t>Not recorded</t>
+        </is>
+      </c>
+      <c r="J17" s="0" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K17" s="0" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N17" s="0">
+        <v>31</v>
+      </c>
+      <c r="O17" s="0">
+        <v>1</v>
+      </c>
+      <c r="P17" s="10">
+        <v>44601.3754282407</v>
+      </c>
+      <c r="Q17" s="0" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
+      <c r="R17" s="0" t="inlineStr">
+        <is>
+          <t>Parrott-Phelan canal trap box</t>
+        </is>
+      </c>
+      <c r="S17" s="0" t="inlineStr">
+        <is>
+          <t>canal trap box</t>
+        </is>
+      </c>
+      <c r="T17" s="0" t="inlineStr">
+        <is>
+          <t>Pigment / dye</t>
+        </is>
+      </c>
+      <c r="U17" s="0" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="V17" s="0" t="inlineStr">
+        <is>
+          <t>Whole body</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="18">
+      <c r="A18" s="0">
+        <v>11</v>
+      </c>
+      <c r="B18" s="0">
+        <v>32475</v>
+      </c>
+      <c r="C18" s="0">
+        <v>1782</v>
+      </c>
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>Chinook salmon</t>
+        </is>
+      </c>
+      <c r="E18" s="0">
+        <v>269</v>
+      </c>
+      <c r="F18" s="0" t="inlineStr">
+        <is>
+          <t>Spring</t>
+        </is>
+      </c>
+      <c r="G18" s="0" t="inlineStr">
+        <is>
+          <t>Spring</t>
+        </is>
+      </c>
+      <c r="H18" s="0" t="inlineStr">
+        <is>
+          <t>Natural</t>
+        </is>
+      </c>
+      <c r="I18" s="0" t="inlineStr">
+        <is>
+          <t>Not recorded</t>
+        </is>
+      </c>
+      <c r="J18" s="0" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K18" s="0" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N18" s="0">
+        <v>46</v>
+      </c>
+      <c r="O18" s="0">
+        <v>1</v>
+      </c>
+      <c r="P18" s="10">
+        <v>44601.4168981481</v>
+      </c>
+      <c r="Q18" s="0" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
+      <c r="R18" s="0" t="inlineStr">
+        <is>
+          <t>Parrot-Phelan RST</t>
+        </is>
+      </c>
+      <c r="S18" s="0" t="inlineStr">
+        <is>
+          <t>PP RST</t>
+        </is>
+      </c>
+      <c r="T18" s="0" t="inlineStr">
+        <is>
+          <t>Pigment / dye</t>
+        </is>
+      </c>
+      <c r="U18" s="0" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="V18" s="0" t="inlineStr">
+        <is>
+          <t>Whole body</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="19">
+      <c r="A19" s="0">
+        <v>11</v>
+      </c>
+      <c r="B19" s="0">
+        <v>33031</v>
+      </c>
+      <c r="C19" s="0">
+        <v>1795</v>
+      </c>
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>Chinook salmon</t>
+        </is>
+      </c>
+      <c r="E19" s="0">
+        <v>270</v>
+      </c>
+      <c r="F19" s="0" t="inlineStr">
+        <is>
+          <t>Spring</t>
+        </is>
+      </c>
+      <c r="G19" s="0" t="inlineStr">
+        <is>
+          <t>Spring</t>
+        </is>
+      </c>
+      <c r="H19" s="0" t="inlineStr">
+        <is>
+          <t>Natural</t>
+        </is>
+      </c>
+      <c r="I19" s="0" t="inlineStr">
+        <is>
+          <t>Not recorded</t>
+        </is>
+      </c>
+      <c r="J19" s="0" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K19" s="0" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N19" s="0">
+        <v>40</v>
+      </c>
+      <c r="O19" s="0">
+        <v>1</v>
+      </c>
+      <c r="P19" s="10">
+        <v>44608.500474537</v>
+      </c>
+      <c r="Q19" s="0" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
+      <c r="R19" s="0" t="inlineStr">
+        <is>
+          <t>Parrot-Phelan RST</t>
+        </is>
+      </c>
+      <c r="S19" s="0" t="inlineStr">
+        <is>
+          <t>PP RST</t>
+        </is>
+      </c>
+      <c r="T19" s="0" t="inlineStr">
+        <is>
+          <t>Pigment / dye</t>
+        </is>
+      </c>
+      <c r="U19" s="0" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="V19" s="0" t="inlineStr">
+        <is>
+          <t>Whole body</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="20">
+      <c r="A20" s="0">
+        <v>11</v>
+      </c>
+      <c r="B20" s="0">
+        <v>33045</v>
+      </c>
+      <c r="C20" s="0">
+        <v>1796</v>
+      </c>
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>Chinook salmon</t>
+        </is>
+      </c>
+      <c r="E20" s="0">
+        <v>270</v>
+      </c>
+      <c r="F20" s="0" t="inlineStr">
+        <is>
+          <t>Spring</t>
+        </is>
+      </c>
+      <c r="H20" s="0" t="inlineStr">
+        <is>
+          <t>Natural</t>
+        </is>
+      </c>
+      <c r="I20" s="0" t="inlineStr">
+        <is>
+          <t>Not recorded</t>
+        </is>
+      </c>
+      <c r="J20" s="0" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K20" s="0" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N20" s="0">
+        <v>21</v>
+      </c>
+      <c r="O20" s="0">
+        <v>1</v>
+      </c>
+      <c r="P20" s="10">
+        <v>44608.3855324074</v>
+      </c>
+      <c r="Q20" s="0" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
+      <c r="R20" s="0" t="inlineStr">
+        <is>
+          <t>Parrott-Phelan canal trap box</t>
+        </is>
+      </c>
+      <c r="S20" s="0" t="inlineStr">
+        <is>
+          <t>canal trap box</t>
+        </is>
+      </c>
+      <c r="T20" s="0" t="inlineStr">
+        <is>
+          <t>Pigment / dye</t>
+        </is>
+      </c>
+      <c r="U20" s="0" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="V20" s="0" t="inlineStr">
+        <is>
+          <t>Whole body</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="21">
+      <c r="A21" s="0">
+        <v>11</v>
+      </c>
+      <c r="B21" s="0">
+        <v>33125</v>
+      </c>
+      <c r="C21" s="0">
+        <v>1797</v>
+      </c>
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>Chinook salmon</t>
+        </is>
+      </c>
+      <c r="E21" s="0">
+        <v>270</v>
+      </c>
+      <c r="F21" s="0" t="inlineStr">
+        <is>
+          <t>Not recorded</t>
+        </is>
+      </c>
+      <c r="G21" s="0" t="inlineStr">
+        <is>
+          <t>Not recorded</t>
+        </is>
+      </c>
+      <c r="H21" s="0" t="inlineStr">
+        <is>
+          <t>Natural</t>
+        </is>
+      </c>
+      <c r="I21" s="0" t="inlineStr">
+        <is>
+          <t>Not recorded</t>
+        </is>
+      </c>
+      <c r="J21" s="0" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K21" s="0" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N21" s="0">
+        <v>9</v>
+      </c>
+      <c r="O21" s="0">
+        <v>1</v>
+      </c>
+      <c r="P21" s="10">
+        <v>44609.4378703704</v>
+      </c>
+      <c r="Q21" s="0" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
+      <c r="R21" s="0" t="inlineStr">
+        <is>
+          <t>Parrot-Phelan RST</t>
+        </is>
+      </c>
+      <c r="S21" s="0" t="inlineStr">
+        <is>
+          <t>PP RST</t>
+        </is>
+      </c>
+      <c r="T21" s="0" t="inlineStr">
+        <is>
+          <t>Pigment / dye</t>
+        </is>
+      </c>
+      <c r="U21" s="0" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="V21" s="0" t="inlineStr">
+        <is>
+          <t>Whole body</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="22">
+      <c r="A22" s="0">
+        <v>11</v>
+      </c>
+      <c r="B22" s="0">
+        <v>33139</v>
+      </c>
+      <c r="C22" s="0">
+        <v>1798</v>
+      </c>
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>Chinook salmon</t>
+        </is>
+      </c>
+      <c r="E22" s="0">
+        <v>270</v>
+      </c>
+      <c r="F22" s="0" t="inlineStr">
+        <is>
+          <t>Spring</t>
+        </is>
+      </c>
+      <c r="H22" s="0" t="inlineStr">
+        <is>
+          <t>Natural</t>
+        </is>
+      </c>
+      <c r="I22" s="0" t="inlineStr">
+        <is>
+          <t>Not recorded</t>
+        </is>
+      </c>
+      <c r="J22" s="0" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K22" s="0" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N22" s="0">
+        <v>11</v>
+      </c>
+      <c r="O22" s="0">
+        <v>1</v>
+      </c>
+      <c r="P22" s="10">
+        <v>44609.3652199074</v>
+      </c>
+      <c r="Q22" s="0" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
+      <c r="R22" s="0" t="inlineStr">
+        <is>
+          <t>Parrott-Phelan canal trap box</t>
+        </is>
+      </c>
+      <c r="S22" s="0" t="inlineStr">
+        <is>
+          <t>canal trap box</t>
+        </is>
+      </c>
+      <c r="T22" s="0" t="inlineStr">
+        <is>
+          <t>Pigment / dye</t>
+        </is>
+      </c>
+      <c r="U22" s="0" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="V22" s="0" t="inlineStr">
+        <is>
+          <t>Whole body</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="23">
+      <c r="A23" s="0">
+        <v>11</v>
+      </c>
+      <c r="B23" s="0">
+        <v>34367</v>
+      </c>
+      <c r="C23" s="0">
+        <v>1837</v>
+      </c>
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>Chinook salmon</t>
+        </is>
+      </c>
+      <c r="E23" s="0">
+        <v>271</v>
+      </c>
+      <c r="F23" s="0" t="inlineStr">
+        <is>
+          <t>Spring</t>
+        </is>
+      </c>
+      <c r="H23" s="0" t="inlineStr">
+        <is>
+          <t>Natural</t>
+        </is>
+      </c>
+      <c r="I23" s="0" t="inlineStr">
+        <is>
+          <t>Not recorded</t>
+        </is>
+      </c>
+      <c r="J23" s="0" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K23" s="0" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N23" s="0">
+        <v>11</v>
+      </c>
+      <c r="O23" s="0">
+        <v>1</v>
+      </c>
+      <c r="P23" s="10">
+        <v>44629.3857407407</v>
+      </c>
+      <c r="Q23" s="0" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
+      <c r="R23" s="0" t="inlineStr">
+        <is>
+          <t>Parrott-Phelan canal trap box</t>
+        </is>
+      </c>
+      <c r="S23" s="0" t="inlineStr">
+        <is>
+          <t>canal trap box</t>
+        </is>
+      </c>
+      <c r="T23" s="0" t="inlineStr">
+        <is>
+          <t>Pigment / dye</t>
+        </is>
+      </c>
+      <c r="U23" s="0" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="V23" s="0" t="inlineStr">
+        <is>
+          <t>Whole body</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="24">
+      <c r="A24" s="0">
+        <v>11</v>
+      </c>
+      <c r="B24" s="0">
+        <v>34395</v>
+      </c>
+      <c r="C24" s="0">
+        <v>1838</v>
+      </c>
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>Chinook salmon</t>
+        </is>
+      </c>
+      <c r="E24" s="0">
+        <v>271</v>
+      </c>
+      <c r="F24" s="0" t="inlineStr">
+        <is>
+          <t>Spring</t>
+        </is>
+      </c>
+      <c r="G24" s="0" t="inlineStr">
+        <is>
+          <t>Spring</t>
+        </is>
+      </c>
+      <c r="H24" s="0" t="inlineStr">
+        <is>
+          <t>Natural</t>
+        </is>
+      </c>
+      <c r="I24" s="0" t="inlineStr">
+        <is>
+          <t>Not recorded</t>
+        </is>
+      </c>
+      <c r="J24" s="0" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K24" s="0" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N24" s="0">
+        <v>12</v>
+      </c>
+      <c r="O24" s="0">
+        <v>1</v>
+      </c>
+      <c r="P24" s="10">
+        <v>44629.4276967593</v>
+      </c>
+      <c r="Q24" s="0" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
+      <c r="R24" s="0" t="inlineStr">
+        <is>
+          <t>Parrot-Phelan RST</t>
+        </is>
+      </c>
+      <c r="S24" s="0" t="inlineStr">
+        <is>
+          <t>PP RST</t>
+        </is>
+      </c>
+      <c r="T24" s="0" t="inlineStr">
+        <is>
+          <t>Pigment / dye</t>
+        </is>
+      </c>
+      <c r="U24" s="0" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="V24" s="0" t="inlineStr">
+        <is>
+          <t>Whole body</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="25">
+      <c r="A25" s="0">
+        <v>11</v>
+      </c>
+      <c r="B25" s="0">
+        <v>34455</v>
+      </c>
+      <c r="C25" s="0">
+        <v>1840</v>
+      </c>
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>Chinook salmon</t>
+        </is>
+      </c>
+      <c r="E25" s="0">
+        <v>271</v>
+      </c>
+      <c r="F25" s="0" t="inlineStr">
+        <is>
+          <t>Spring</t>
+        </is>
+      </c>
+      <c r="G25" s="0" t="inlineStr">
+        <is>
+          <t>Spring</t>
+        </is>
+      </c>
+      <c r="H25" s="0" t="inlineStr">
+        <is>
+          <t>Natural</t>
+        </is>
+      </c>
+      <c r="I25" s="0" t="inlineStr">
+        <is>
+          <t>Not recorded</t>
+        </is>
+      </c>
+      <c r="J25" s="0" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K25" s="0" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N25" s="0">
+        <v>4</v>
+      </c>
+      <c r="O25" s="0">
+        <v>1</v>
+      </c>
+      <c r="P25" s="10">
+        <v>44630.4167939815</v>
+      </c>
+      <c r="Q25" s="0" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
+      <c r="R25" s="0" t="inlineStr">
+        <is>
+          <t>Parrot-Phelan RST</t>
+        </is>
+      </c>
+      <c r="S25" s="0" t="inlineStr">
+        <is>
+          <t>PP RST</t>
+        </is>
+      </c>
+      <c r="T25" s="0" t="inlineStr">
+        <is>
+          <t>Pigment / dye</t>
+        </is>
+      </c>
+      <c r="U25" s="0" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="V25" s="0" t="inlineStr">
+        <is>
+          <t>Whole body</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="26">
+      <c r="A26" s="0">
+        <v>11</v>
+      </c>
+      <c r="B26" s="0">
+        <v>37670</v>
+      </c>
+      <c r="C26" s="0">
+        <v>1784</v>
+      </c>
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>Chinook salmon</t>
+        </is>
+      </c>
+      <c r="E26" s="0">
+        <v>269</v>
+      </c>
+      <c r="F26" s="0" t="inlineStr">
+        <is>
+          <t>Not recorded</t>
+        </is>
+      </c>
+      <c r="G26" s="0" t="inlineStr">
+        <is>
+          <t>Not recorded</t>
+        </is>
+      </c>
+      <c r="H26" s="0" t="inlineStr">
+        <is>
+          <t>Natural</t>
+        </is>
+      </c>
+      <c r="I26" s="0" t="inlineStr">
+        <is>
+          <t>Not recorded</t>
+        </is>
+      </c>
+      <c r="J26" s="0" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K26" s="0" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N26" s="0">
+        <v>6</v>
+      </c>
+      <c r="O26" s="0">
+        <v>1</v>
+      </c>
+      <c r="P26" s="10">
+        <v>44602.4168055556</v>
+      </c>
+      <c r="Q26" s="0" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
+      <c r="R26" s="0" t="inlineStr">
+        <is>
+          <t>Parrot-Phelan RST</t>
+        </is>
+      </c>
+      <c r="S26" s="0" t="inlineStr">
+        <is>
+          <t>PP RST</t>
+        </is>
+      </c>
+      <c r="T26" s="0" t="inlineStr">
+        <is>
+          <t>Pigment / dye</t>
+        </is>
+      </c>
+      <c r="U26" s="0" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="V26" s="0" t="inlineStr">
+        <is>
+          <t>Whole body</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="27">
+      <c r="A27" s="0">
+        <v>11</v>
+      </c>
+      <c r="B27" s="0">
+        <v>37671</v>
+      </c>
+      <c r="C27" s="0">
+        <v>1786</v>
+      </c>
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>Chinook salmon</t>
+        </is>
+      </c>
+      <c r="E27" s="0">
+        <v>269</v>
+      </c>
+      <c r="F27" s="0" t="inlineStr">
+        <is>
+          <t>Spring</t>
+        </is>
+      </c>
+      <c r="H27" s="0" t="inlineStr">
+        <is>
+          <t>Natural</t>
+        </is>
+      </c>
+      <c r="I27" s="0" t="inlineStr">
+        <is>
+          <t>Not recorded</t>
+        </is>
+      </c>
+      <c r="J27" s="0" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K27" s="0" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="N27" s="0">
+        <v>1</v>
+      </c>
+      <c r="O27" s="0">
+        <v>1</v>
+      </c>
+      <c r="P27" s="10">
+        <v>44603.3860763889</v>
+      </c>
+      <c r="Q27" s="0" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
+      <c r="R27" s="0" t="inlineStr">
+        <is>
+          <t>Parrott-Phelan canal trap box</t>
+        </is>
+      </c>
+      <c r="S27" s="0" t="inlineStr">
+        <is>
+          <t>canal trap box</t>
+        </is>
+      </c>
+      <c r="T27" s="0" t="inlineStr">
+        <is>
+          <t>Pigment / dye</t>
+        </is>
+      </c>
+      <c r="U27" s="0" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="V27" s="0" t="inlineStr">
+        <is>
+          <t>Whole body</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updates files with new query from grant
</commit_message>
<xml_diff>
--- a/data-raw/butte_recapture_edi.xlsx
+++ b/data-raw/butte_recapture_edi.xlsx
@@ -8,10 +8,10 @@
   </bookViews>
   <sheets>
     <sheet sheetId="1" r:id="rId1" name="Recapture EDI"/>
-    <sheet r:id="rId4" name="Recapture_EDI" sheetId="2"/>
+    <sheet r:id="rId4" sheetId="2" name="Recapture_EDI"/>
   </sheets>
   <definedNames>
-    <definedName name="Recapture_EDI">'Recapture_EDI'!$A$1:$W$27</definedName>
+    <definedName name="Recapture_EDI">'Recapture_EDI'!$A$1:$V$16</definedName>
   </definedNames>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
@@ -2950,74 +2950,70 @@
       </c>
       <c r="J1" s="0" t="inlineStr">
         <is>
-          <t>mort</t>
+          <t>actualCount</t>
         </is>
       </c>
       <c r="K1" s="0" t="inlineStr">
         <is>
-          <t>actualCount</t>
+          <t>forkLength</t>
         </is>
       </c>
       <c r="L1" s="0" t="inlineStr">
         <is>
-          <t>forkLength</t>
+          <t>totalLength</t>
         </is>
       </c>
       <c r="M1" s="0" t="inlineStr">
         <is>
-          <t>totalLength</t>
+          <t>n</t>
         </is>
       </c>
       <c r="N1" s="0" t="inlineStr">
         <is>
-          <t>n</t>
+          <t>actualCountID</t>
         </is>
       </c>
       <c r="O1" s="0" t="inlineStr">
         <is>
-          <t>actualCountID</t>
+          <t>visitTime</t>
         </is>
       </c>
       <c r="P1" s="0" t="inlineStr">
         <is>
-          <t>visitTime</t>
+          <t>visitType</t>
         </is>
       </c>
       <c r="Q1" s="0" t="inlineStr">
         <is>
-          <t>visitType</t>
+          <t>siteName</t>
         </is>
       </c>
       <c r="R1" s="0" t="inlineStr">
         <is>
-          <t>siteName</t>
+          <t>subSiteName</t>
         </is>
       </c>
       <c r="S1" s="0" t="inlineStr">
         <is>
-          <t>subSiteName</t>
+          <t>markType</t>
         </is>
       </c>
       <c r="T1" s="0" t="inlineStr">
         <is>
-          <t>markType</t>
+          <t>markColor</t>
         </is>
       </c>
       <c r="U1" s="0" t="inlineStr">
         <is>
-          <t>markColor</t>
+          <t>markPosition</t>
         </is>
       </c>
       <c r="V1" s="0" t="inlineStr">
         <is>
-          <t>markPosition</t>
-        </is>
-      </c>
-      <c r="W1" s="0" t="inlineStr">
-        <is>
           <t>markCode</t>
         </is>
       </c>
+      <c r="W1" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="2">
       <c r="A2" s="0">
@@ -3054,53 +3050,50 @@
       </c>
       <c r="J2" s="0" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K2" s="0" t="inlineStr">
-        <is>
           <t>Yes</t>
         </is>
+      </c>
+      <c r="K2" s="0" t="inlineStr"/>
+      <c r="M2" s="0">
+        <v>1</v>
       </c>
       <c r="N2" s="0">
         <v>1</v>
       </c>
       <c r="O2" s="0">
-        <v>1</v>
-      </c>
-      <c r="P2" s="10">
         <v>44213.3964236111</v>
       </c>
+      <c r="P2" s="10" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
       <c r="Q2" s="0" t="inlineStr">
         <is>
-          <t>Continue trapping</t>
+          <t>Parrot-Phelan RST</t>
         </is>
       </c>
       <c r="R2" s="0" t="inlineStr">
         <is>
-          <t>Parrot-Phelan RST</t>
+          <t>PP RST</t>
         </is>
       </c>
       <c r="S2" s="0" t="inlineStr">
         <is>
-          <t>PP RST</t>
+          <t>Pigment / dye</t>
         </is>
       </c>
       <c r="T2" s="0" t="inlineStr">
         <is>
-          <t>Pigment / dye</t>
+          <t>Brown</t>
         </is>
       </c>
       <c r="U2" s="0" t="inlineStr">
         <is>
-          <t>Brown</t>
-        </is>
-      </c>
-      <c r="V2" s="0" t="inlineStr">
-        <is>
           <t>Whole body</t>
         </is>
       </c>
+      <c r="V2" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="3">
       <c r="A3" s="0">
@@ -3137,53 +3130,50 @@
       </c>
       <c r="J3" s="0" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K3" s="0" t="inlineStr">
-        <is>
           <t>Yes</t>
         </is>
       </c>
+      <c r="K3" s="0" t="inlineStr"/>
+      <c r="M3" s="0">
+        <v>10</v>
+      </c>
       <c r="N3" s="0">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="O3" s="0">
-        <v>1</v>
-      </c>
-      <c r="P3" s="10">
         <v>44238.3755439815</v>
       </c>
+      <c r="P3" s="10" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
       <c r="Q3" s="0" t="inlineStr">
         <is>
-          <t>Continue trapping</t>
+          <t>Parrot-Phelan RST</t>
         </is>
       </c>
       <c r="R3" s="0" t="inlineStr">
         <is>
-          <t>Parrot-Phelan RST</t>
+          <t>PP RST</t>
         </is>
       </c>
       <c r="S3" s="0" t="inlineStr">
         <is>
-          <t>PP RST</t>
+          <t>Pigment / dye</t>
         </is>
       </c>
       <c r="T3" s="0" t="inlineStr">
         <is>
-          <t>Pigment / dye</t>
+          <t>Brown</t>
         </is>
       </c>
       <c r="U3" s="0" t="inlineStr">
         <is>
-          <t>Brown</t>
-        </is>
-      </c>
-      <c r="V3" s="0" t="inlineStr">
-        <is>
           <t>Whole body</t>
         </is>
       </c>
+      <c r="V3" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="4">
       <c r="A4" s="0">
@@ -3220,53 +3210,50 @@
       </c>
       <c r="J4" s="0" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K4" s="0" t="inlineStr">
-        <is>
           <t>Yes</t>
         </is>
       </c>
+      <c r="K4" s="0" t="inlineStr"/>
+      <c r="M4" s="0">
+        <v>8</v>
+      </c>
       <c r="N4" s="0">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="O4" s="0">
-        <v>1</v>
-      </c>
-      <c r="P4" s="10">
         <v>44239.6459143519</v>
       </c>
+      <c r="P4" s="10" t="inlineStr">
+        <is>
+          <t>Unplanned restart</t>
+        </is>
+      </c>
       <c r="Q4" s="0" t="inlineStr">
         <is>
-          <t>Unplanned restart</t>
+          <t>Parrot-Phelan RST</t>
         </is>
       </c>
       <c r="R4" s="0" t="inlineStr">
         <is>
-          <t>Parrot-Phelan RST</t>
+          <t>PP RST</t>
         </is>
       </c>
       <c r="S4" s="0" t="inlineStr">
         <is>
-          <t>PP RST</t>
+          <t>Pigment / dye</t>
         </is>
       </c>
       <c r="T4" s="0" t="inlineStr">
         <is>
-          <t>Pigment / dye</t>
+          <t>Brown</t>
         </is>
       </c>
       <c r="U4" s="0" t="inlineStr">
         <is>
-          <t>Brown</t>
-        </is>
-      </c>
-      <c r="V4" s="0" t="inlineStr">
-        <is>
           <t>Whole body</t>
         </is>
       </c>
+      <c r="V4" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="5">
       <c r="A5" s="0">
@@ -3303,53 +3290,50 @@
       </c>
       <c r="J5" s="0" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K5" s="0" t="inlineStr">
-        <is>
           <t>Yes</t>
         </is>
       </c>
+      <c r="K5" s="0" t="inlineStr"/>
+      <c r="M5" s="0">
+        <v>65</v>
+      </c>
       <c r="N5" s="0">
-        <v>65</v>
+        <v>1</v>
       </c>
       <c r="O5" s="0">
-        <v>1</v>
-      </c>
-      <c r="P5" s="10">
         <v>44252.3962037037</v>
       </c>
+      <c r="P5" s="10" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
       <c r="Q5" s="0" t="inlineStr">
         <is>
-          <t>Continue trapping</t>
+          <t>Parrot-Phelan RST</t>
         </is>
       </c>
       <c r="R5" s="0" t="inlineStr">
         <is>
-          <t>Parrot-Phelan RST</t>
+          <t>PP RST</t>
         </is>
       </c>
       <c r="S5" s="0" t="inlineStr">
         <is>
-          <t>PP RST</t>
+          <t>Pigment / dye</t>
         </is>
       </c>
       <c r="T5" s="0" t="inlineStr">
         <is>
-          <t>Pigment / dye</t>
+          <t>Brown</t>
         </is>
       </c>
       <c r="U5" s="0" t="inlineStr">
         <is>
-          <t>Brown</t>
-        </is>
-      </c>
-      <c r="V5" s="0" t="inlineStr">
-        <is>
           <t>Whole body</t>
         </is>
       </c>
+      <c r="V5" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="6">
       <c r="A6" s="0">
@@ -3386,53 +3370,50 @@
       </c>
       <c r="J6" s="0" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K6" s="0" t="inlineStr">
-        <is>
           <t>Yes</t>
         </is>
       </c>
+      <c r="K6" s="0" t="inlineStr"/>
+      <c r="M6" s="0">
+        <v>24</v>
+      </c>
       <c r="N6" s="0">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="O6" s="0">
-        <v>1</v>
-      </c>
-      <c r="P6" s="10">
         <v>44253.3755902778</v>
       </c>
+      <c r="P6" s="10" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
       <c r="Q6" s="0" t="inlineStr">
         <is>
-          <t>Continue trapping</t>
+          <t>Parrot-Phelan RST</t>
         </is>
       </c>
       <c r="R6" s="0" t="inlineStr">
         <is>
-          <t>Parrot-Phelan RST</t>
+          <t>PP RST</t>
         </is>
       </c>
       <c r="S6" s="0" t="inlineStr">
         <is>
-          <t>PP RST</t>
+          <t>Pigment / dye</t>
         </is>
       </c>
       <c r="T6" s="0" t="inlineStr">
         <is>
-          <t>Pigment / dye</t>
+          <t>Brown</t>
         </is>
       </c>
       <c r="U6" s="0" t="inlineStr">
         <is>
-          <t>Brown</t>
-        </is>
-      </c>
-      <c r="V6" s="0" t="inlineStr">
-        <is>
           <t>Whole body</t>
         </is>
       </c>
+      <c r="V6" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="7">
       <c r="A7" s="0">
@@ -3469,53 +3450,50 @@
       </c>
       <c r="J7" s="0" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K7" s="0" t="inlineStr">
-        <is>
           <t>Yes</t>
         </is>
       </c>
+      <c r="K7" s="0" t="inlineStr"/>
+      <c r="M7" s="0">
+        <v>13</v>
+      </c>
       <c r="N7" s="0">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="O7" s="0">
-        <v>1</v>
-      </c>
-      <c r="P7" s="10">
         <v>44266.4030324074</v>
       </c>
+      <c r="P7" s="10" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
       <c r="Q7" s="0" t="inlineStr">
         <is>
-          <t>Continue trapping</t>
+          <t>Parrot-Phelan RST</t>
         </is>
       </c>
       <c r="R7" s="0" t="inlineStr">
         <is>
-          <t>Parrot-Phelan RST</t>
+          <t>PP RST</t>
         </is>
       </c>
       <c r="S7" s="0" t="inlineStr">
         <is>
-          <t>PP RST</t>
+          <t>Pigment / dye</t>
         </is>
       </c>
       <c r="T7" s="0" t="inlineStr">
         <is>
-          <t>Pigment / dye</t>
+          <t>Brown</t>
         </is>
       </c>
       <c r="U7" s="0" t="inlineStr">
         <is>
-          <t>Brown</t>
-        </is>
-      </c>
-      <c r="V7" s="0" t="inlineStr">
-        <is>
           <t>Whole body</t>
         </is>
       </c>
+      <c r="V7" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="8">
       <c r="A8" s="0">
@@ -3552,53 +3530,50 @@
       </c>
       <c r="J8" s="0" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K8" s="0" t="inlineStr">
-        <is>
           <t>Yes</t>
         </is>
       </c>
+      <c r="K8" s="0" t="inlineStr"/>
+      <c r="M8" s="0">
+        <v>6</v>
+      </c>
       <c r="N8" s="0">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="O8" s="0">
-        <v>1</v>
-      </c>
-      <c r="P8" s="10">
         <v>44267.3755787037</v>
       </c>
+      <c r="P8" s="10" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
       <c r="Q8" s="0" t="inlineStr">
         <is>
-          <t>Continue trapping</t>
+          <t>Parrot-Phelan RST</t>
         </is>
       </c>
       <c r="R8" s="0" t="inlineStr">
         <is>
-          <t>Parrot-Phelan RST</t>
+          <t>PP RST</t>
         </is>
       </c>
       <c r="S8" s="0" t="inlineStr">
         <is>
-          <t>PP RST</t>
+          <t>Pigment / dye</t>
         </is>
       </c>
       <c r="T8" s="0" t="inlineStr">
         <is>
-          <t>Pigment / dye</t>
+          <t>Brown</t>
         </is>
       </c>
       <c r="U8" s="0" t="inlineStr">
         <is>
-          <t>Brown</t>
-        </is>
-      </c>
-      <c r="V8" s="0" t="inlineStr">
-        <is>
           <t>Whole body</t>
         </is>
       </c>
+      <c r="V8" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="9">
       <c r="A9" s="0">
@@ -3635,53 +3610,50 @@
       </c>
       <c r="J9" s="0" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K9" s="0" t="inlineStr">
-        <is>
           <t>Yes</t>
         </is>
       </c>
+      <c r="K9" s="0" t="inlineStr"/>
+      <c r="M9" s="0">
+        <v>6</v>
+      </c>
       <c r="N9" s="0">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="O9" s="0">
-        <v>1</v>
-      </c>
-      <c r="P9" s="10">
         <v>44295.4794916088</v>
       </c>
+      <c r="P9" s="10" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
       <c r="Q9" s="0" t="inlineStr">
         <is>
-          <t>Continue trapping</t>
+          <t>Parrot-Phelan RST</t>
         </is>
       </c>
       <c r="R9" s="0" t="inlineStr">
         <is>
-          <t>Parrot-Phelan RST</t>
+          <t>PP RST</t>
         </is>
       </c>
       <c r="S9" s="0" t="inlineStr">
         <is>
-          <t>PP RST</t>
+          <t>Pigment / dye</t>
         </is>
       </c>
       <c r="T9" s="0" t="inlineStr">
         <is>
-          <t>Pigment / dye</t>
+          <t>Brown</t>
         </is>
       </c>
       <c r="U9" s="0" t="inlineStr">
         <is>
-          <t>Brown</t>
-        </is>
-      </c>
-      <c r="V9" s="0" t="inlineStr">
-        <is>
           <t>Whole body</t>
         </is>
       </c>
+      <c r="V9" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="10">
       <c r="A10" s="0">
@@ -3718,53 +3690,50 @@
       </c>
       <c r="J10" s="0" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K10" s="0" t="inlineStr">
-        <is>
           <t>Yes</t>
         </is>
       </c>
+      <c r="K10" s="0" t="inlineStr"/>
+      <c r="M10" s="0">
+        <v>109</v>
+      </c>
       <c r="N10" s="0">
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="O10" s="0">
-        <v>1</v>
-      </c>
-      <c r="P10" s="10">
         <v>44302.4375231481</v>
       </c>
+      <c r="P10" s="10" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
       <c r="Q10" s="0" t="inlineStr">
         <is>
-          <t>Continue trapping</t>
+          <t>Parrot-Phelan RST</t>
         </is>
       </c>
       <c r="R10" s="0" t="inlineStr">
         <is>
-          <t>Parrot-Phelan RST</t>
+          <t>PP RST</t>
         </is>
       </c>
       <c r="S10" s="0" t="inlineStr">
         <is>
-          <t>PP RST</t>
+          <t>Pigment / dye</t>
         </is>
       </c>
       <c r="T10" s="0" t="inlineStr">
         <is>
-          <t>Pigment / dye</t>
+          <t>Brown</t>
         </is>
       </c>
       <c r="U10" s="0" t="inlineStr">
         <is>
-          <t>Brown</t>
-        </is>
-      </c>
-      <c r="V10" s="0" t="inlineStr">
-        <is>
           <t>Whole body</t>
         </is>
       </c>
+      <c r="V10" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="11">
       <c r="A11" s="0">
@@ -3801,53 +3770,50 @@
       </c>
       <c r="J11" s="0" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K11" s="0" t="inlineStr">
-        <is>
           <t>Yes</t>
         </is>
       </c>
+      <c r="K11" s="0" t="inlineStr"/>
+      <c r="M11" s="0">
+        <v>3</v>
+      </c>
       <c r="N11" s="0">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O11" s="0">
-        <v>1</v>
-      </c>
-      <c r="P11" s="10">
         <v>44303.4665583681</v>
       </c>
+      <c r="P11" s="10" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
       <c r="Q11" s="0" t="inlineStr">
         <is>
-          <t>Continue trapping</t>
+          <t>Parrot-Phelan RST</t>
         </is>
       </c>
       <c r="R11" s="0" t="inlineStr">
         <is>
-          <t>Parrot-Phelan RST</t>
+          <t>PP RST</t>
         </is>
       </c>
       <c r="S11" s="0" t="inlineStr">
         <is>
-          <t>PP RST</t>
+          <t>Pigment / dye</t>
         </is>
       </c>
       <c r="T11" s="0" t="inlineStr">
         <is>
-          <t>Pigment / dye</t>
+          <t>Brown</t>
         </is>
       </c>
       <c r="U11" s="0" t="inlineStr">
         <is>
-          <t>Brown</t>
-        </is>
-      </c>
-      <c r="V11" s="0" t="inlineStr">
-        <is>
           <t>Whole body</t>
         </is>
       </c>
+      <c r="V11" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="12">
       <c r="A12" s="0">
@@ -3884,53 +3850,50 @@
       </c>
       <c r="J12" s="0" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K12" s="0" t="inlineStr">
-        <is>
           <t>Yes</t>
         </is>
       </c>
+      <c r="K12" s="0" t="inlineStr"/>
+      <c r="M12" s="0">
+        <v>14</v>
+      </c>
       <c r="N12" s="0">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="O12" s="0">
-        <v>1</v>
-      </c>
-      <c r="P12" s="10">
         <v>44203.4376967593</v>
       </c>
+      <c r="P12" s="10" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
       <c r="Q12" s="0" t="inlineStr">
         <is>
-          <t>Continue trapping</t>
+          <t>Parrot-Phelan RST</t>
         </is>
       </c>
       <c r="R12" s="0" t="inlineStr">
         <is>
-          <t>Parrot-Phelan RST</t>
+          <t>PP RST</t>
         </is>
       </c>
       <c r="S12" s="0" t="inlineStr">
         <is>
-          <t>PP RST</t>
+          <t>Pigment / dye</t>
         </is>
       </c>
       <c r="T12" s="0" t="inlineStr">
         <is>
-          <t>Pigment / dye</t>
+          <t>Brown</t>
         </is>
       </c>
       <c r="U12" s="0" t="inlineStr">
         <is>
-          <t>Brown</t>
-        </is>
-      </c>
-      <c r="V12" s="0" t="inlineStr">
-        <is>
           <t>Whole body</t>
         </is>
       </c>
+      <c r="V12" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="13">
       <c r="A13" s="0">
@@ -3967,53 +3930,50 @@
       </c>
       <c r="J13" s="0" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K13" s="0" t="inlineStr">
-        <is>
           <t>Yes</t>
         </is>
       </c>
+      <c r="K13" s="0" t="inlineStr"/>
+      <c r="M13" s="0">
+        <v>5</v>
+      </c>
       <c r="N13" s="0">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="O13" s="0">
-        <v>1</v>
-      </c>
-      <c r="P13" s="10">
         <v>44204.3959606482</v>
       </c>
+      <c r="P13" s="10" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
       <c r="Q13" s="0" t="inlineStr">
         <is>
-          <t>Continue trapping</t>
+          <t>Parrot-Phelan RST</t>
         </is>
       </c>
       <c r="R13" s="0" t="inlineStr">
         <is>
-          <t>Parrot-Phelan RST</t>
+          <t>PP RST</t>
         </is>
       </c>
       <c r="S13" s="0" t="inlineStr">
         <is>
-          <t>PP RST</t>
+          <t>Pigment / dye</t>
         </is>
       </c>
       <c r="T13" s="0" t="inlineStr">
         <is>
-          <t>Pigment / dye</t>
+          <t>Brown</t>
         </is>
       </c>
       <c r="U13" s="0" t="inlineStr">
         <is>
-          <t>Brown</t>
-        </is>
-      </c>
-      <c r="V13" s="0" t="inlineStr">
-        <is>
           <t>Whole body</t>
         </is>
       </c>
+      <c r="V13" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="14">
       <c r="A14" s="0">
@@ -4050,53 +4010,50 @@
       </c>
       <c r="J14" s="0" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K14" s="0" t="inlineStr">
-        <is>
           <t>Yes</t>
         </is>
       </c>
+      <c r="K14" s="0" t="inlineStr"/>
+      <c r="M14" s="0">
+        <v>3</v>
+      </c>
       <c r="N14" s="0">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O14" s="0">
-        <v>1</v>
-      </c>
-      <c r="P14" s="10">
         <v>44205.416712963</v>
       </c>
+      <c r="P14" s="10" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
       <c r="Q14" s="0" t="inlineStr">
         <is>
-          <t>Continue trapping</t>
+          <t>Parrot-Phelan RST</t>
         </is>
       </c>
       <c r="R14" s="0" t="inlineStr">
         <is>
-          <t>Parrot-Phelan RST</t>
+          <t>PP RST</t>
         </is>
       </c>
       <c r="S14" s="0" t="inlineStr">
         <is>
-          <t>PP RST</t>
+          <t>Pigment / dye</t>
         </is>
       </c>
       <c r="T14" s="0" t="inlineStr">
         <is>
-          <t>Pigment / dye</t>
+          <t>Brown</t>
         </is>
       </c>
       <c r="U14" s="0" t="inlineStr">
         <is>
-          <t>Brown</t>
-        </is>
-      </c>
-      <c r="V14" s="0" t="inlineStr">
-        <is>
           <t>Whole body</t>
         </is>
       </c>
+      <c r="V14" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="15">
       <c r="A15" s="0">
@@ -4133,53 +4090,50 @@
       </c>
       <c r="J15" s="0" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K15" s="0" t="inlineStr">
-        <is>
           <t>Yes</t>
         </is>
       </c>
+      <c r="K15" s="0" t="inlineStr"/>
+      <c r="M15" s="0">
+        <v>55</v>
+      </c>
       <c r="N15" s="0">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="O15" s="0">
-        <v>1</v>
-      </c>
-      <c r="P15" s="10">
         <v>44211.5833449074</v>
       </c>
+      <c r="P15" s="10" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
       <c r="Q15" s="0" t="inlineStr">
         <is>
-          <t>Continue trapping</t>
+          <t>Parrot-Phelan RST</t>
         </is>
       </c>
       <c r="R15" s="0" t="inlineStr">
         <is>
-          <t>Parrot-Phelan RST</t>
+          <t>PP RST</t>
         </is>
       </c>
       <c r="S15" s="0" t="inlineStr">
         <is>
-          <t>PP RST</t>
+          <t>Pigment / dye</t>
         </is>
       </c>
       <c r="T15" s="0" t="inlineStr">
         <is>
-          <t>Pigment / dye</t>
+          <t>Brown</t>
         </is>
       </c>
       <c r="U15" s="0" t="inlineStr">
         <is>
-          <t>Brown</t>
-        </is>
-      </c>
-      <c r="V15" s="0" t="inlineStr">
-        <is>
           <t>Whole body</t>
         </is>
       </c>
+      <c r="V15" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="16">
       <c r="A16" s="0">
@@ -4216,996 +4170,287 @@
       </c>
       <c r="J16" s="0" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K16" s="0" t="inlineStr">
-        <is>
           <t>Yes</t>
         </is>
       </c>
+      <c r="K16" s="0" t="inlineStr"/>
+      <c r="M16" s="0">
+        <v>5</v>
+      </c>
       <c r="N16" s="0">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="O16" s="0">
-        <v>1</v>
-      </c>
-      <c r="P16" s="10">
         <v>44212.3750462963</v>
       </c>
+      <c r="P16" s="10" t="inlineStr">
+        <is>
+          <t>Continue trapping</t>
+        </is>
+      </c>
       <c r="Q16" s="0" t="inlineStr">
         <is>
-          <t>Continue trapping</t>
+          <t>Parrot-Phelan RST</t>
         </is>
       </c>
       <c r="R16" s="0" t="inlineStr">
         <is>
-          <t>Parrot-Phelan RST</t>
+          <t>PP RST</t>
         </is>
       </c>
       <c r="S16" s="0" t="inlineStr">
         <is>
-          <t>PP RST</t>
+          <t>Pigment / dye</t>
         </is>
       </c>
       <c r="T16" s="0" t="inlineStr">
         <is>
-          <t>Pigment / dye</t>
+          <t>Brown</t>
         </is>
       </c>
       <c r="U16" s="0" t="inlineStr">
         <is>
-          <t>Brown</t>
-        </is>
-      </c>
-      <c r="V16" s="0" t="inlineStr">
-        <is>
           <t>Whole body</t>
         </is>
       </c>
+      <c r="V16" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="17">
-      <c r="A17" s="0">
-        <v>11</v>
-      </c>
-      <c r="B17" s="0">
-        <v>32454</v>
-      </c>
-      <c r="C17" s="0">
-        <v>1781</v>
-      </c>
-      <c r="D17" s="0" t="inlineStr">
-        <is>
-          <t>Chinook salmon</t>
-        </is>
-      </c>
-      <c r="E17" s="0">
-        <v>269</v>
-      </c>
-      <c r="F17" s="0" t="inlineStr">
-        <is>
-          <t>Spring</t>
-        </is>
-      </c>
-      <c r="H17" s="0" t="inlineStr">
-        <is>
-          <t>Natural</t>
-        </is>
-      </c>
-      <c r="I17" s="0" t="inlineStr">
-        <is>
-          <t>Not recorded</t>
-        </is>
-      </c>
-      <c r="J17" s="0" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K17" s="0" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="N17" s="0">
-        <v>31</v>
-      </c>
-      <c r="O17" s="0">
-        <v>1</v>
-      </c>
-      <c r="P17" s="10">
-        <v>44601.3754282407</v>
-      </c>
-      <c r="Q17" s="0" t="inlineStr">
-        <is>
-          <t>Continue trapping</t>
-        </is>
-      </c>
-      <c r="R17" s="0" t="inlineStr">
-        <is>
-          <t>Parrott-Phelan canal trap box</t>
-        </is>
-      </c>
-      <c r="S17" s="0" t="inlineStr">
-        <is>
-          <t>canal trap box</t>
-        </is>
-      </c>
-      <c r="T17" s="0" t="inlineStr">
-        <is>
-          <t>Pigment / dye</t>
-        </is>
-      </c>
-      <c r="U17" s="0" t="inlineStr">
-        <is>
-          <t>Brown</t>
-        </is>
-      </c>
-      <c r="V17" s="0" t="inlineStr">
-        <is>
-          <t>Whole body</t>
-        </is>
-      </c>
+      <c r="A17" s="0"/>
+      <c r="B17" s="0"/>
+      <c r="C17" s="0"/>
+      <c r="D17" s="0" t="inlineStr"/>
+      <c r="E17" s="0"/>
+      <c r="F17" s="0" t="inlineStr"/>
+      <c r="H17" s="0" t="inlineStr"/>
+      <c r="I17" s="0" t="inlineStr"/>
+      <c r="J17" s="0" t="inlineStr"/>
+      <c r="K17" s="0" t="inlineStr"/>
+      <c r="N17" s="0"/>
+      <c r="O17" s="0"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="0" t="inlineStr"/>
+      <c r="R17" s="0" t="inlineStr"/>
+      <c r="S17" s="0" t="inlineStr"/>
+      <c r="T17" s="0" t="inlineStr"/>
+      <c r="U17" s="0" t="inlineStr"/>
+      <c r="V17" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="18">
-      <c r="A18" s="0">
-        <v>11</v>
-      </c>
-      <c r="B18" s="0">
-        <v>32475</v>
-      </c>
-      <c r="C18" s="0">
-        <v>1782</v>
-      </c>
-      <c r="D18" s="0" t="inlineStr">
-        <is>
-          <t>Chinook salmon</t>
-        </is>
-      </c>
-      <c r="E18" s="0">
-        <v>269</v>
-      </c>
-      <c r="F18" s="0" t="inlineStr">
-        <is>
-          <t>Spring</t>
-        </is>
-      </c>
-      <c r="G18" s="0" t="inlineStr">
-        <is>
-          <t>Spring</t>
-        </is>
-      </c>
-      <c r="H18" s="0" t="inlineStr">
-        <is>
-          <t>Natural</t>
-        </is>
-      </c>
-      <c r="I18" s="0" t="inlineStr">
-        <is>
-          <t>Not recorded</t>
-        </is>
-      </c>
-      <c r="J18" s="0" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K18" s="0" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="N18" s="0">
-        <v>46</v>
-      </c>
-      <c r="O18" s="0">
-        <v>1</v>
-      </c>
-      <c r="P18" s="10">
-        <v>44601.4168981481</v>
-      </c>
-      <c r="Q18" s="0" t="inlineStr">
-        <is>
-          <t>Continue trapping</t>
-        </is>
-      </c>
-      <c r="R18" s="0" t="inlineStr">
-        <is>
-          <t>Parrot-Phelan RST</t>
-        </is>
-      </c>
-      <c r="S18" s="0" t="inlineStr">
-        <is>
-          <t>PP RST</t>
-        </is>
-      </c>
-      <c r="T18" s="0" t="inlineStr">
-        <is>
-          <t>Pigment / dye</t>
-        </is>
-      </c>
-      <c r="U18" s="0" t="inlineStr">
-        <is>
-          <t>Brown</t>
-        </is>
-      </c>
-      <c r="V18" s="0" t="inlineStr">
-        <is>
-          <t>Whole body</t>
-        </is>
-      </c>
+      <c r="A18" s="0"/>
+      <c r="B18" s="0"/>
+      <c r="C18" s="0"/>
+      <c r="D18" s="0" t="inlineStr"/>
+      <c r="E18" s="0"/>
+      <c r="F18" s="0" t="inlineStr"/>
+      <c r="G18" s="0" t="inlineStr"/>
+      <c r="H18" s="0" t="inlineStr"/>
+      <c r="I18" s="0" t="inlineStr"/>
+      <c r="J18" s="0" t="inlineStr"/>
+      <c r="K18" s="0" t="inlineStr"/>
+      <c r="N18" s="0"/>
+      <c r="O18" s="0"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="0" t="inlineStr"/>
+      <c r="R18" s="0" t="inlineStr"/>
+      <c r="S18" s="0" t="inlineStr"/>
+      <c r="T18" s="0" t="inlineStr"/>
+      <c r="U18" s="0" t="inlineStr"/>
+      <c r="V18" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="19">
-      <c r="A19" s="0">
-        <v>11</v>
-      </c>
-      <c r="B19" s="0">
-        <v>33031</v>
-      </c>
-      <c r="C19" s="0">
-        <v>1795</v>
-      </c>
-      <c r="D19" s="0" t="inlineStr">
-        <is>
-          <t>Chinook salmon</t>
-        </is>
-      </c>
-      <c r="E19" s="0">
-        <v>270</v>
-      </c>
-      <c r="F19" s="0" t="inlineStr">
-        <is>
-          <t>Spring</t>
-        </is>
-      </c>
-      <c r="G19" s="0" t="inlineStr">
-        <is>
-          <t>Spring</t>
-        </is>
-      </c>
-      <c r="H19" s="0" t="inlineStr">
-        <is>
-          <t>Natural</t>
-        </is>
-      </c>
-      <c r="I19" s="0" t="inlineStr">
-        <is>
-          <t>Not recorded</t>
-        </is>
-      </c>
-      <c r="J19" s="0" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K19" s="0" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="N19" s="0">
-        <v>40</v>
-      </c>
-      <c r="O19" s="0">
-        <v>1</v>
-      </c>
-      <c r="P19" s="10">
-        <v>44608.500474537</v>
-      </c>
-      <c r="Q19" s="0" t="inlineStr">
-        <is>
-          <t>Continue trapping</t>
-        </is>
-      </c>
-      <c r="R19" s="0" t="inlineStr">
-        <is>
-          <t>Parrot-Phelan RST</t>
-        </is>
-      </c>
-      <c r="S19" s="0" t="inlineStr">
-        <is>
-          <t>PP RST</t>
-        </is>
-      </c>
-      <c r="T19" s="0" t="inlineStr">
-        <is>
-          <t>Pigment / dye</t>
-        </is>
-      </c>
-      <c r="U19" s="0" t="inlineStr">
-        <is>
-          <t>Brown</t>
-        </is>
-      </c>
-      <c r="V19" s="0" t="inlineStr">
-        <is>
-          <t>Whole body</t>
-        </is>
-      </c>
+      <c r="A19" s="0"/>
+      <c r="B19" s="0"/>
+      <c r="C19" s="0"/>
+      <c r="D19" s="0" t="inlineStr"/>
+      <c r="E19" s="0"/>
+      <c r="F19" s="0" t="inlineStr"/>
+      <c r="G19" s="0" t="inlineStr"/>
+      <c r="H19" s="0" t="inlineStr"/>
+      <c r="I19" s="0" t="inlineStr"/>
+      <c r="J19" s="0" t="inlineStr"/>
+      <c r="K19" s="0" t="inlineStr"/>
+      <c r="N19" s="0"/>
+      <c r="O19" s="0"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="0" t="inlineStr"/>
+      <c r="R19" s="0" t="inlineStr"/>
+      <c r="S19" s="0" t="inlineStr"/>
+      <c r="T19" s="0" t="inlineStr"/>
+      <c r="U19" s="0" t="inlineStr"/>
+      <c r="V19" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="20">
-      <c r="A20" s="0">
-        <v>11</v>
-      </c>
-      <c r="B20" s="0">
-        <v>33045</v>
-      </c>
-      <c r="C20" s="0">
-        <v>1796</v>
-      </c>
-      <c r="D20" s="0" t="inlineStr">
-        <is>
-          <t>Chinook salmon</t>
-        </is>
-      </c>
-      <c r="E20" s="0">
-        <v>270</v>
-      </c>
-      <c r="F20" s="0" t="inlineStr">
-        <is>
-          <t>Spring</t>
-        </is>
-      </c>
-      <c r="H20" s="0" t="inlineStr">
-        <is>
-          <t>Natural</t>
-        </is>
-      </c>
-      <c r="I20" s="0" t="inlineStr">
-        <is>
-          <t>Not recorded</t>
-        </is>
-      </c>
-      <c r="J20" s="0" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K20" s="0" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="N20" s="0">
-        <v>21</v>
-      </c>
-      <c r="O20" s="0">
-        <v>1</v>
-      </c>
-      <c r="P20" s="10">
-        <v>44608.3855324074</v>
-      </c>
-      <c r="Q20" s="0" t="inlineStr">
-        <is>
-          <t>Continue trapping</t>
-        </is>
-      </c>
-      <c r="R20" s="0" t="inlineStr">
-        <is>
-          <t>Parrott-Phelan canal trap box</t>
-        </is>
-      </c>
-      <c r="S20" s="0" t="inlineStr">
-        <is>
-          <t>canal trap box</t>
-        </is>
-      </c>
-      <c r="T20" s="0" t="inlineStr">
-        <is>
-          <t>Pigment / dye</t>
-        </is>
-      </c>
-      <c r="U20" s="0" t="inlineStr">
-        <is>
-          <t>Brown</t>
-        </is>
-      </c>
-      <c r="V20" s="0" t="inlineStr">
-        <is>
-          <t>Whole body</t>
-        </is>
-      </c>
+      <c r="A20" s="0"/>
+      <c r="B20" s="0"/>
+      <c r="C20" s="0"/>
+      <c r="D20" s="0" t="inlineStr"/>
+      <c r="E20" s="0"/>
+      <c r="F20" s="0" t="inlineStr"/>
+      <c r="H20" s="0" t="inlineStr"/>
+      <c r="I20" s="0" t="inlineStr"/>
+      <c r="J20" s="0" t="inlineStr"/>
+      <c r="K20" s="0" t="inlineStr"/>
+      <c r="N20" s="0"/>
+      <c r="O20" s="0"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="0" t="inlineStr"/>
+      <c r="R20" s="0" t="inlineStr"/>
+      <c r="S20" s="0" t="inlineStr"/>
+      <c r="T20" s="0" t="inlineStr"/>
+      <c r="U20" s="0" t="inlineStr"/>
+      <c r="V20" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="21">
-      <c r="A21" s="0">
-        <v>11</v>
-      </c>
-      <c r="B21" s="0">
-        <v>33125</v>
-      </c>
-      <c r="C21" s="0">
-        <v>1797</v>
-      </c>
-      <c r="D21" s="0" t="inlineStr">
-        <is>
-          <t>Chinook salmon</t>
-        </is>
-      </c>
-      <c r="E21" s="0">
-        <v>270</v>
-      </c>
-      <c r="F21" s="0" t="inlineStr">
-        <is>
-          <t>Not recorded</t>
-        </is>
-      </c>
-      <c r="G21" s="0" t="inlineStr">
-        <is>
-          <t>Not recorded</t>
-        </is>
-      </c>
-      <c r="H21" s="0" t="inlineStr">
-        <is>
-          <t>Natural</t>
-        </is>
-      </c>
-      <c r="I21" s="0" t="inlineStr">
-        <is>
-          <t>Not recorded</t>
-        </is>
-      </c>
-      <c r="J21" s="0" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K21" s="0" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="N21" s="0">
-        <v>9</v>
-      </c>
-      <c r="O21" s="0">
-        <v>1</v>
-      </c>
-      <c r="P21" s="10">
-        <v>44609.4378703704</v>
-      </c>
-      <c r="Q21" s="0" t="inlineStr">
-        <is>
-          <t>Continue trapping</t>
-        </is>
-      </c>
-      <c r="R21" s="0" t="inlineStr">
-        <is>
-          <t>Parrot-Phelan RST</t>
-        </is>
-      </c>
-      <c r="S21" s="0" t="inlineStr">
-        <is>
-          <t>PP RST</t>
-        </is>
-      </c>
-      <c r="T21" s="0" t="inlineStr">
-        <is>
-          <t>Pigment / dye</t>
-        </is>
-      </c>
-      <c r="U21" s="0" t="inlineStr">
-        <is>
-          <t>Brown</t>
-        </is>
-      </c>
-      <c r="V21" s="0" t="inlineStr">
-        <is>
-          <t>Whole body</t>
-        </is>
-      </c>
+      <c r="A21" s="0"/>
+      <c r="B21" s="0"/>
+      <c r="C21" s="0"/>
+      <c r="D21" s="0" t="inlineStr"/>
+      <c r="E21" s="0"/>
+      <c r="F21" s="0" t="inlineStr"/>
+      <c r="G21" s="0" t="inlineStr"/>
+      <c r="H21" s="0" t="inlineStr"/>
+      <c r="I21" s="0" t="inlineStr"/>
+      <c r="J21" s="0" t="inlineStr"/>
+      <c r="K21" s="0" t="inlineStr"/>
+      <c r="N21" s="0"/>
+      <c r="O21" s="0"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="0" t="inlineStr"/>
+      <c r="R21" s="0" t="inlineStr"/>
+      <c r="S21" s="0" t="inlineStr"/>
+      <c r="T21" s="0" t="inlineStr"/>
+      <c r="U21" s="0" t="inlineStr"/>
+      <c r="V21" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="22">
-      <c r="A22" s="0">
-        <v>11</v>
-      </c>
-      <c r="B22" s="0">
-        <v>33139</v>
-      </c>
-      <c r="C22" s="0">
-        <v>1798</v>
-      </c>
-      <c r="D22" s="0" t="inlineStr">
-        <is>
-          <t>Chinook salmon</t>
-        </is>
-      </c>
-      <c r="E22" s="0">
-        <v>270</v>
-      </c>
-      <c r="F22" s="0" t="inlineStr">
-        <is>
-          <t>Spring</t>
-        </is>
-      </c>
-      <c r="H22" s="0" t="inlineStr">
-        <is>
-          <t>Natural</t>
-        </is>
-      </c>
-      <c r="I22" s="0" t="inlineStr">
-        <is>
-          <t>Not recorded</t>
-        </is>
-      </c>
-      <c r="J22" s="0" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K22" s="0" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="N22" s="0">
-        <v>11</v>
-      </c>
-      <c r="O22" s="0">
-        <v>1</v>
-      </c>
-      <c r="P22" s="10">
-        <v>44609.3652199074</v>
-      </c>
-      <c r="Q22" s="0" t="inlineStr">
-        <is>
-          <t>Continue trapping</t>
-        </is>
-      </c>
-      <c r="R22" s="0" t="inlineStr">
-        <is>
-          <t>Parrott-Phelan canal trap box</t>
-        </is>
-      </c>
-      <c r="S22" s="0" t="inlineStr">
-        <is>
-          <t>canal trap box</t>
-        </is>
-      </c>
-      <c r="T22" s="0" t="inlineStr">
-        <is>
-          <t>Pigment / dye</t>
-        </is>
-      </c>
-      <c r="U22" s="0" t="inlineStr">
-        <is>
-          <t>Brown</t>
-        </is>
-      </c>
-      <c r="V22" s="0" t="inlineStr">
-        <is>
-          <t>Whole body</t>
-        </is>
-      </c>
+      <c r="A22" s="0"/>
+      <c r="B22" s="0"/>
+      <c r="C22" s="0"/>
+      <c r="D22" s="0" t="inlineStr"/>
+      <c r="E22" s="0"/>
+      <c r="F22" s="0" t="inlineStr"/>
+      <c r="H22" s="0" t="inlineStr"/>
+      <c r="I22" s="0" t="inlineStr"/>
+      <c r="J22" s="0" t="inlineStr"/>
+      <c r="K22" s="0" t="inlineStr"/>
+      <c r="N22" s="0"/>
+      <c r="O22" s="0"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="0" t="inlineStr"/>
+      <c r="R22" s="0" t="inlineStr"/>
+      <c r="S22" s="0" t="inlineStr"/>
+      <c r="T22" s="0" t="inlineStr"/>
+      <c r="U22" s="0" t="inlineStr"/>
+      <c r="V22" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="23">
-      <c r="A23" s="0">
-        <v>11</v>
-      </c>
-      <c r="B23" s="0">
-        <v>34367</v>
-      </c>
-      <c r="C23" s="0">
-        <v>1837</v>
-      </c>
-      <c r="D23" s="0" t="inlineStr">
-        <is>
-          <t>Chinook salmon</t>
-        </is>
-      </c>
-      <c r="E23" s="0">
-        <v>271</v>
-      </c>
-      <c r="F23" s="0" t="inlineStr">
-        <is>
-          <t>Spring</t>
-        </is>
-      </c>
-      <c r="H23" s="0" t="inlineStr">
-        <is>
-          <t>Natural</t>
-        </is>
-      </c>
-      <c r="I23" s="0" t="inlineStr">
-        <is>
-          <t>Not recorded</t>
-        </is>
-      </c>
-      <c r="J23" s="0" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K23" s="0" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="N23" s="0">
-        <v>11</v>
-      </c>
-      <c r="O23" s="0">
-        <v>1</v>
-      </c>
-      <c r="P23" s="10">
-        <v>44629.3857407407</v>
-      </c>
-      <c r="Q23" s="0" t="inlineStr">
-        <is>
-          <t>Continue trapping</t>
-        </is>
-      </c>
-      <c r="R23" s="0" t="inlineStr">
-        <is>
-          <t>Parrott-Phelan canal trap box</t>
-        </is>
-      </c>
-      <c r="S23" s="0" t="inlineStr">
-        <is>
-          <t>canal trap box</t>
-        </is>
-      </c>
-      <c r="T23" s="0" t="inlineStr">
-        <is>
-          <t>Pigment / dye</t>
-        </is>
-      </c>
-      <c r="U23" s="0" t="inlineStr">
-        <is>
-          <t>Brown</t>
-        </is>
-      </c>
-      <c r="V23" s="0" t="inlineStr">
-        <is>
-          <t>Whole body</t>
-        </is>
-      </c>
+      <c r="A23" s="0"/>
+      <c r="B23" s="0"/>
+      <c r="C23" s="0"/>
+      <c r="D23" s="0" t="inlineStr"/>
+      <c r="E23" s="0"/>
+      <c r="F23" s="0" t="inlineStr"/>
+      <c r="H23" s="0" t="inlineStr"/>
+      <c r="I23" s="0" t="inlineStr"/>
+      <c r="J23" s="0" t="inlineStr"/>
+      <c r="K23" s="0" t="inlineStr"/>
+      <c r="N23" s="0"/>
+      <c r="O23" s="0"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="0" t="inlineStr"/>
+      <c r="R23" s="0" t="inlineStr"/>
+      <c r="S23" s="0" t="inlineStr"/>
+      <c r="T23" s="0" t="inlineStr"/>
+      <c r="U23" s="0" t="inlineStr"/>
+      <c r="V23" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="24">
-      <c r="A24" s="0">
-        <v>11</v>
-      </c>
-      <c r="B24" s="0">
-        <v>34395</v>
-      </c>
-      <c r="C24" s="0">
-        <v>1838</v>
-      </c>
-      <c r="D24" s="0" t="inlineStr">
-        <is>
-          <t>Chinook salmon</t>
-        </is>
-      </c>
-      <c r="E24" s="0">
-        <v>271</v>
-      </c>
-      <c r="F24" s="0" t="inlineStr">
-        <is>
-          <t>Spring</t>
-        </is>
-      </c>
-      <c r="G24" s="0" t="inlineStr">
-        <is>
-          <t>Spring</t>
-        </is>
-      </c>
-      <c r="H24" s="0" t="inlineStr">
-        <is>
-          <t>Natural</t>
-        </is>
-      </c>
-      <c r="I24" s="0" t="inlineStr">
-        <is>
-          <t>Not recorded</t>
-        </is>
-      </c>
-      <c r="J24" s="0" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K24" s="0" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="N24" s="0">
-        <v>12</v>
-      </c>
-      <c r="O24" s="0">
-        <v>1</v>
-      </c>
-      <c r="P24" s="10">
-        <v>44629.4276967593</v>
-      </c>
-      <c r="Q24" s="0" t="inlineStr">
-        <is>
-          <t>Continue trapping</t>
-        </is>
-      </c>
-      <c r="R24" s="0" t="inlineStr">
-        <is>
-          <t>Parrot-Phelan RST</t>
-        </is>
-      </c>
-      <c r="S24" s="0" t="inlineStr">
-        <is>
-          <t>PP RST</t>
-        </is>
-      </c>
-      <c r="T24" s="0" t="inlineStr">
-        <is>
-          <t>Pigment / dye</t>
-        </is>
-      </c>
-      <c r="U24" s="0" t="inlineStr">
-        <is>
-          <t>Brown</t>
-        </is>
-      </c>
-      <c r="V24" s="0" t="inlineStr">
-        <is>
-          <t>Whole body</t>
-        </is>
-      </c>
+      <c r="A24" s="0"/>
+      <c r="B24" s="0"/>
+      <c r="C24" s="0"/>
+      <c r="D24" s="0" t="inlineStr"/>
+      <c r="E24" s="0"/>
+      <c r="F24" s="0" t="inlineStr"/>
+      <c r="G24" s="0" t="inlineStr"/>
+      <c r="H24" s="0" t="inlineStr"/>
+      <c r="I24" s="0" t="inlineStr"/>
+      <c r="J24" s="0" t="inlineStr"/>
+      <c r="K24" s="0" t="inlineStr"/>
+      <c r="N24" s="0"/>
+      <c r="O24" s="0"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="0" t="inlineStr"/>
+      <c r="R24" s="0" t="inlineStr"/>
+      <c r="S24" s="0" t="inlineStr"/>
+      <c r="T24" s="0" t="inlineStr"/>
+      <c r="U24" s="0" t="inlineStr"/>
+      <c r="V24" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="25">
-      <c r="A25" s="0">
-        <v>11</v>
-      </c>
-      <c r="B25" s="0">
-        <v>34455</v>
-      </c>
-      <c r="C25" s="0">
-        <v>1840</v>
-      </c>
-      <c r="D25" s="0" t="inlineStr">
-        <is>
-          <t>Chinook salmon</t>
-        </is>
-      </c>
-      <c r="E25" s="0">
-        <v>271</v>
-      </c>
-      <c r="F25" s="0" t="inlineStr">
-        <is>
-          <t>Spring</t>
-        </is>
-      </c>
-      <c r="G25" s="0" t="inlineStr">
-        <is>
-          <t>Spring</t>
-        </is>
-      </c>
-      <c r="H25" s="0" t="inlineStr">
-        <is>
-          <t>Natural</t>
-        </is>
-      </c>
-      <c r="I25" s="0" t="inlineStr">
-        <is>
-          <t>Not recorded</t>
-        </is>
-      </c>
-      <c r="J25" s="0" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K25" s="0" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="N25" s="0">
-        <v>4</v>
-      </c>
-      <c r="O25" s="0">
-        <v>1</v>
-      </c>
-      <c r="P25" s="10">
-        <v>44630.4167939815</v>
-      </c>
-      <c r="Q25" s="0" t="inlineStr">
-        <is>
-          <t>Continue trapping</t>
-        </is>
-      </c>
-      <c r="R25" s="0" t="inlineStr">
-        <is>
-          <t>Parrot-Phelan RST</t>
-        </is>
-      </c>
-      <c r="S25" s="0" t="inlineStr">
-        <is>
-          <t>PP RST</t>
-        </is>
-      </c>
-      <c r="T25" s="0" t="inlineStr">
-        <is>
-          <t>Pigment / dye</t>
-        </is>
-      </c>
-      <c r="U25" s="0" t="inlineStr">
-        <is>
-          <t>Brown</t>
-        </is>
-      </c>
-      <c r="V25" s="0" t="inlineStr">
-        <is>
-          <t>Whole body</t>
-        </is>
-      </c>
+      <c r="A25" s="0"/>
+      <c r="B25" s="0"/>
+      <c r="C25" s="0"/>
+      <c r="D25" s="0" t="inlineStr"/>
+      <c r="E25" s="0"/>
+      <c r="F25" s="0" t="inlineStr"/>
+      <c r="G25" s="0" t="inlineStr"/>
+      <c r="H25" s="0" t="inlineStr"/>
+      <c r="I25" s="0" t="inlineStr"/>
+      <c r="J25" s="0" t="inlineStr"/>
+      <c r="K25" s="0" t="inlineStr"/>
+      <c r="N25" s="0"/>
+      <c r="O25" s="0"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="0" t="inlineStr"/>
+      <c r="R25" s="0" t="inlineStr"/>
+      <c r="S25" s="0" t="inlineStr"/>
+      <c r="T25" s="0" t="inlineStr"/>
+      <c r="U25" s="0" t="inlineStr"/>
+      <c r="V25" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="26">
-      <c r="A26" s="0">
-        <v>11</v>
-      </c>
-      <c r="B26" s="0">
-        <v>37670</v>
-      </c>
-      <c r="C26" s="0">
-        <v>1784</v>
-      </c>
-      <c r="D26" s="0" t="inlineStr">
-        <is>
-          <t>Chinook salmon</t>
-        </is>
-      </c>
-      <c r="E26" s="0">
-        <v>269</v>
-      </c>
-      <c r="F26" s="0" t="inlineStr">
-        <is>
-          <t>Not recorded</t>
-        </is>
-      </c>
-      <c r="G26" s="0" t="inlineStr">
-        <is>
-          <t>Not recorded</t>
-        </is>
-      </c>
-      <c r="H26" s="0" t="inlineStr">
-        <is>
-          <t>Natural</t>
-        </is>
-      </c>
-      <c r="I26" s="0" t="inlineStr">
-        <is>
-          <t>Not recorded</t>
-        </is>
-      </c>
-      <c r="J26" s="0" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K26" s="0" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="N26" s="0">
-        <v>6</v>
-      </c>
-      <c r="O26" s="0">
-        <v>1</v>
-      </c>
-      <c r="P26" s="10">
-        <v>44602.4168055556</v>
-      </c>
-      <c r="Q26" s="0" t="inlineStr">
-        <is>
-          <t>Continue trapping</t>
-        </is>
-      </c>
-      <c r="R26" s="0" t="inlineStr">
-        <is>
-          <t>Parrot-Phelan RST</t>
-        </is>
-      </c>
-      <c r="S26" s="0" t="inlineStr">
-        <is>
-          <t>PP RST</t>
-        </is>
-      </c>
-      <c r="T26" s="0" t="inlineStr">
-        <is>
-          <t>Pigment / dye</t>
-        </is>
-      </c>
-      <c r="U26" s="0" t="inlineStr">
-        <is>
-          <t>Brown</t>
-        </is>
-      </c>
-      <c r="V26" s="0" t="inlineStr">
-        <is>
-          <t>Whole body</t>
-        </is>
-      </c>
+      <c r="A26" s="0"/>
+      <c r="B26" s="0"/>
+      <c r="C26" s="0"/>
+      <c r="D26" s="0" t="inlineStr"/>
+      <c r="E26" s="0"/>
+      <c r="F26" s="0" t="inlineStr"/>
+      <c r="G26" s="0" t="inlineStr"/>
+      <c r="H26" s="0" t="inlineStr"/>
+      <c r="I26" s="0" t="inlineStr"/>
+      <c r="J26" s="0" t="inlineStr"/>
+      <c r="K26" s="0" t="inlineStr"/>
+      <c r="N26" s="0"/>
+      <c r="O26" s="0"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="0" t="inlineStr"/>
+      <c r="R26" s="0" t="inlineStr"/>
+      <c r="S26" s="0" t="inlineStr"/>
+      <c r="T26" s="0" t="inlineStr"/>
+      <c r="U26" s="0" t="inlineStr"/>
+      <c r="V26" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="27">
-      <c r="A27" s="0">
-        <v>11</v>
-      </c>
-      <c r="B27" s="0">
-        <v>37671</v>
-      </c>
-      <c r="C27" s="0">
-        <v>1786</v>
-      </c>
-      <c r="D27" s="0" t="inlineStr">
-        <is>
-          <t>Chinook salmon</t>
-        </is>
-      </c>
-      <c r="E27" s="0">
-        <v>269</v>
-      </c>
-      <c r="F27" s="0" t="inlineStr">
-        <is>
-          <t>Spring</t>
-        </is>
-      </c>
-      <c r="H27" s="0" t="inlineStr">
-        <is>
-          <t>Natural</t>
-        </is>
-      </c>
-      <c r="I27" s="0" t="inlineStr">
-        <is>
-          <t>Not recorded</t>
-        </is>
-      </c>
-      <c r="J27" s="0" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K27" s="0" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="N27" s="0">
-        <v>1</v>
-      </c>
-      <c r="O27" s="0">
-        <v>1</v>
-      </c>
-      <c r="P27" s="10">
-        <v>44603.3860763889</v>
-      </c>
-      <c r="Q27" s="0" t="inlineStr">
-        <is>
-          <t>Continue trapping</t>
-        </is>
-      </c>
-      <c r="R27" s="0" t="inlineStr">
-        <is>
-          <t>Parrott-Phelan canal trap box</t>
-        </is>
-      </c>
-      <c r="S27" s="0" t="inlineStr">
-        <is>
-          <t>canal trap box</t>
-        </is>
-      </c>
-      <c r="T27" s="0" t="inlineStr">
-        <is>
-          <t>Pigment / dye</t>
-        </is>
-      </c>
-      <c r="U27" s="0" t="inlineStr">
-        <is>
-          <t>Brown</t>
-        </is>
-      </c>
-      <c r="V27" s="0" t="inlineStr">
-        <is>
-          <t>Whole body</t>
-        </is>
-      </c>
+      <c r="A27" s="0"/>
+      <c r="B27" s="0"/>
+      <c r="C27" s="0"/>
+      <c r="D27" s="0" t="inlineStr"/>
+      <c r="E27" s="0"/>
+      <c r="F27" s="0" t="inlineStr"/>
+      <c r="H27" s="0" t="inlineStr"/>
+      <c r="I27" s="0" t="inlineStr"/>
+      <c r="J27" s="0" t="inlineStr"/>
+      <c r="K27" s="0" t="inlineStr"/>
+      <c r="N27" s="0"/>
+      <c r="O27" s="0"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="0" t="inlineStr"/>
+      <c r="R27" s="0" t="inlineStr"/>
+      <c r="S27" s="0" t="inlineStr"/>
+      <c r="T27" s="0" t="inlineStr"/>
+      <c r="U27" s="0" t="inlineStr"/>
+      <c r="V27" s="0" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>